<commit_message>
update Accounting and linksPage
</commit_message>
<xml_diff>
--- a/linksPage.xlsx
+++ b/linksPage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15760" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15680" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="linkTable" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="170">
   <si>
     <t>request</t>
   </si>
@@ -535,10 +535,13 @@
     <t>"ok" / "false" / "wrongRequest"</t>
   </si>
   <si>
-    <t>"ok" / "false" / "wrongRequest" / "noSendEmail</t>
-  </si>
-  <si>
-    <t>"ok" / "noSendEmail / "wrongRequest"</t>
+    <t>"ok" / "noSendEmail / "wrongRequest" / "wrongCredentials"</t>
+  </si>
+  <si>
+    <t>"ok" / "false" / "wrongRequest" / "noSendEmail" / "wrongCredentials"</t>
+  </si>
+  <si>
+    <t>"ok" / "false" / "wrongRequest" / "wrongCredentials"</t>
   </si>
 </sst>
 </file>
@@ -962,66 +965,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1029,11 +972,71 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="237">
@@ -1653,13 +1656,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="35" t="s">
         <v>147</v>
       </c>
       <c r="D2" s="15" t="s">
@@ -1670,9 +1673,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="32"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
       <c r="D3" s="15" t="s">
         <v>2</v>
       </c>
@@ -1681,9 +1684,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1">
-      <c r="A4" s="32"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
       <c r="D4" s="15" t="s">
         <v>4</v>
       </c>
@@ -1692,9 +1695,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1">
-      <c r="A5" s="32"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
       <c r="D5" s="15" t="s">
         <v>5</v>
       </c>
@@ -1703,59 +1706,59 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1">
-      <c r="A6" s="32"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
       <c r="E6" s="15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="37" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="33" t="s">
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="37" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
-      <c r="A8" s="33"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="33"/>
+      <c r="E8" s="37"/>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="37" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
       <c r="E9" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1">
-      <c r="A10" s="33"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
       <c r="E10" s="1" t="s">
         <v>28</v>
       </c>
@@ -1776,13 +1779,13 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="35" t="s">
         <v>104</v>
       </c>
       <c r="D12" s="15" t="s">
@@ -1793,9 +1796,9 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1">
-      <c r="A13" s="32"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
+      <c r="A13" s="36"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
       <c r="D13" s="15" t="s">
         <v>5</v>
       </c>
@@ -1804,9 +1807,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1">
-      <c r="A14" s="32"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
+      <c r="A14" s="36"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
       <c r="D14" s="15" t="s">
         <v>7</v>
       </c>
@@ -1821,62 +1824,62 @@
       <c r="B15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
       <c r="E15" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="37" t="s">
         <v>39</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
       <c r="E16" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1">
-      <c r="A17" s="33"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
       <c r="E17" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1">
-      <c r="A18" s="33" t="s">
+      <c r="A18" s="37" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="C18" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1">
-      <c r="A19" s="33"/>
+      <c r="A19" s="37"/>
       <c r="B19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
       <c r="E19" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="36" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="15" t="s">
@@ -1893,88 +1896,88 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1">
-      <c r="A21" s="32"/>
+      <c r="A21" s="36"/>
       <c r="B21" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
       <c r="E21" s="15" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1">
-      <c r="A22" s="32"/>
+      <c r="A22" s="36"/>
       <c r="B22" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
       <c r="E22" s="15" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1">
-      <c r="A23" s="32"/>
+      <c r="A23" s="36"/>
       <c r="B23" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
       <c r="E23" s="15" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1">
-      <c r="A24" s="32"/>
+      <c r="A24" s="36"/>
       <c r="B24" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
       <c r="E24" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1">
-      <c r="A25" s="32"/>
+      <c r="A25" s="36"/>
       <c r="B25" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
       <c r="E25" s="15" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1">
-      <c r="A26" s="32"/>
+      <c r="A26" s="36"/>
       <c r="B26" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
       <c r="E26" s="15" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1">
-      <c r="A27" s="32"/>
+      <c r="A27" s="36"/>
       <c r="B27" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
       <c r="E27" s="15" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" customHeight="1">
-      <c r="A28" s="32"/>
-      <c r="B28" s="34" t="s">
+      <c r="A28" s="36"/>
+      <c r="B28" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="34" t="s">
+      <c r="C28" s="35" t="s">
         <v>117</v>
       </c>
       <c r="D28" s="16" t="s">
@@ -1985,9 +1988,9 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" customHeight="1">
-      <c r="A29" s="32"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
+      <c r="A29" s="36"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
       <c r="D29" s="15" t="s">
         <v>7</v>
       </c>
@@ -1996,11 +1999,11 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" customHeight="1">
-      <c r="A30" s="32"/>
-      <c r="B30" s="34" t="s">
+      <c r="A30" s="36"/>
+      <c r="B30" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="34" t="s">
+      <c r="C30" s="35" t="s">
         <v>118</v>
       </c>
       <c r="D30" s="15" t="s">
@@ -2011,9 +2014,9 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="15" customHeight="1">
-      <c r="A31" s="32"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
+      <c r="A31" s="36"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="35"/>
       <c r="D31" s="15" t="s">
         <v>7</v>
       </c>
@@ -2022,11 +2025,11 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" customHeight="1">
-      <c r="A32" s="32"/>
-      <c r="B32" s="34" t="s">
+      <c r="A32" s="36"/>
+      <c r="B32" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="35" t="s">
         <v>119</v>
       </c>
       <c r="D32" s="15" t="s">
@@ -2037,9 +2040,9 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" customHeight="1">
-      <c r="A33" s="32"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
+      <c r="A33" s="36"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="35"/>
       <c r="D33" s="15" t="s">
         <v>7</v>
       </c>
@@ -2048,13 +2051,13 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" customHeight="1">
-      <c r="A34" s="33" t="s">
+      <c r="A34" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="B34" s="33" t="s">
+      <c r="B34" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="33" t="s">
+      <c r="C34" s="37" t="s">
         <v>106</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -2065,9 +2068,9 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" customHeight="1">
-      <c r="A35" s="33"/>
-      <c r="B35" s="33"/>
-      <c r="C35" s="33"/>
+      <c r="A35" s="37"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
       <c r="D35" s="1" t="s">
         <v>7</v>
       </c>
@@ -2076,48 +2079,48 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" customHeight="1">
-      <c r="A36" s="33"/>
+      <c r="A36" s="37"/>
       <c r="B36" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
       <c r="E36" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" customHeight="1">
-      <c r="A37" s="33" t="s">
+      <c r="A37" s="37" t="s">
         <v>56</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="36" t="s">
+      <c r="C37" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
     </row>
     <row r="38" spans="1:5" ht="15" customHeight="1">
-      <c r="A38" s="33"/>
+      <c r="A38" s="37"/>
       <c r="B38" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
       <c r="E38" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15" customHeight="1">
-      <c r="A39" s="33" t="s">
+      <c r="A39" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="33" t="s">
+      <c r="B39" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="33" t="s">
+      <c r="C39" s="37" t="s">
         <v>107</v>
       </c>
       <c r="D39" s="1" t="s">
@@ -2128,9 +2131,9 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="15" customHeight="1">
-      <c r="A40" s="33"/>
-      <c r="B40" s="33"/>
-      <c r="C40" s="33"/>
+      <c r="A40" s="37"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="37"/>
       <c r="D40" s="1" t="s">
         <v>7</v>
       </c>
@@ -2139,13 +2142,13 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="15" customHeight="1">
-      <c r="A41" s="33" t="s">
+      <c r="A41" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="B41" s="33" t="s">
+      <c r="B41" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="C41" s="33" t="s">
+      <c r="C41" s="37" t="s">
         <v>120</v>
       </c>
       <c r="D41" s="1" t="s">
@@ -2156,9 +2159,9 @@
       </c>
     </row>
     <row r="42" spans="1:5" ht="15" customHeight="1">
-      <c r="A42" s="33"/>
-      <c r="B42" s="33"/>
-      <c r="C42" s="33"/>
+      <c r="A42" s="37"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="37"/>
       <c r="D42" s="1" t="s">
         <v>7</v>
       </c>
@@ -2167,24 +2170,24 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" customHeight="1">
-      <c r="A43" s="33"/>
+      <c r="A43" s="37"/>
       <c r="B43" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
       <c r="E43" s="1" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15" customHeight="1">
-      <c r="A44" s="32" t="s">
+      <c r="A44" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="B44" s="34" t="s">
+      <c r="B44" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="34" t="s">
+      <c r="C44" s="35" t="s">
         <v>108</v>
       </c>
       <c r="D44" s="15" t="s">
@@ -2195,9 +2198,9 @@
       </c>
     </row>
     <row r="45" spans="1:5" ht="15" customHeight="1">
-      <c r="A45" s="32"/>
-      <c r="B45" s="34"/>
-      <c r="C45" s="34"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="35"/>
       <c r="D45" s="15" t="s">
         <v>7</v>
       </c>
@@ -2206,53 +2209,53 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="15" customHeight="1">
-      <c r="A46" s="32"/>
+      <c r="A46" s="36"/>
       <c r="B46" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C46" s="30"/>
-      <c r="D46" s="30"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="40"/>
       <c r="E46" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15" customHeight="1">
-      <c r="A47" s="32"/>
+      <c r="A47" s="36"/>
       <c r="B47" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C47" s="30"/>
-      <c r="D47" s="30"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="40"/>
       <c r="E47" s="15" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15" customHeight="1">
-      <c r="A48" s="33" t="s">
+      <c r="A48" s="37" t="s">
         <v>45</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C48" s="35" t="s">
+      <c r="C48" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="D48" s="35"/>
-      <c r="E48" s="35"/>
+      <c r="D48" s="39"/>
+      <c r="E48" s="39"/>
     </row>
     <row r="49" spans="1:5" ht="15" customHeight="1">
-      <c r="A49" s="33"/>
+      <c r="A49" s="37"/>
       <c r="B49" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="35"/>
-      <c r="D49" s="35"/>
+      <c r="C49" s="39"/>
+      <c r="D49" s="39"/>
       <c r="E49" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="30" customHeight="1">
-      <c r="A50" s="32" t="s">
+      <c r="A50" s="36" t="s">
         <v>87</v>
       </c>
       <c r="B50" s="15" t="s">
@@ -2269,11 +2272,11 @@
       </c>
     </row>
     <row r="51" spans="1:5" ht="15" customHeight="1">
-      <c r="A51" s="32"/>
-      <c r="B51" s="34" t="s">
+      <c r="A51" s="36"/>
+      <c r="B51" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="C51" s="38" t="s">
+      <c r="C51" s="34" t="s">
         <v>110</v>
       </c>
       <c r="D51" s="17" t="s">
@@ -2284,9 +2287,9 @@
       </c>
     </row>
     <row r="52" spans="1:5" ht="15" customHeight="1">
-      <c r="A52" s="32"/>
-      <c r="B52" s="34"/>
-      <c r="C52" s="38"/>
+      <c r="A52" s="36"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="34"/>
       <c r="D52" s="17" t="s">
         <v>7</v>
       </c>
@@ -2295,7 +2298,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" ht="15" customHeight="1">
-      <c r="A53" s="32" t="s">
+      <c r="A53" s="36" t="s">
         <v>8</v>
       </c>
       <c r="B53" s="15" t="s">
@@ -2312,33 +2315,33 @@
       </c>
     </row>
     <row r="54" spans="1:5" ht="15" customHeight="1">
-      <c r="A54" s="32"/>
+      <c r="A54" s="36"/>
       <c r="B54" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C54" s="30"/>
-      <c r="D54" s="30"/>
+      <c r="C54" s="40"/>
+      <c r="D54" s="40"/>
       <c r="E54" s="15" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15" customHeight="1">
-      <c r="A55" s="32"/>
+      <c r="A55" s="36"/>
       <c r="B55" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="30"/>
-      <c r="D55" s="30"/>
+      <c r="C55" s="40"/>
+      <c r="D55" s="40"/>
       <c r="E55" s="15" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15" customHeight="1">
-      <c r="A56" s="32"/>
-      <c r="B56" s="34" t="s">
+      <c r="A56" s="36"/>
+      <c r="B56" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C56" s="34" t="s">
+      <c r="C56" s="35" t="s">
         <v>112</v>
       </c>
       <c r="D56" s="15" t="s">
@@ -2349,9 +2352,9 @@
       </c>
     </row>
     <row r="57" spans="1:5" ht="15" customHeight="1">
-      <c r="A57" s="32"/>
-      <c r="B57" s="34"/>
-      <c r="C57" s="34"/>
+      <c r="A57" s="36"/>
+      <c r="B57" s="35"/>
+      <c r="C57" s="35"/>
       <c r="D57" s="15" t="s">
         <v>7</v>
       </c>
@@ -2360,35 +2363,35 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="15" customHeight="1">
-      <c r="A58" s="32"/>
+      <c r="A58" s="36"/>
       <c r="B58" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C58" s="30"/>
-      <c r="D58" s="30"/>
+      <c r="C58" s="40"/>
+      <c r="D58" s="40"/>
       <c r="E58" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15" customHeight="1">
-      <c r="A59" s="32"/>
+      <c r="A59" s="36"/>
       <c r="B59" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C59" s="30"/>
-      <c r="D59" s="30"/>
+      <c r="C59" s="40"/>
+      <c r="D59" s="40"/>
       <c r="E59" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15" customHeight="1">
-      <c r="A60" s="33" t="s">
+      <c r="A60" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="B60" s="33" t="s">
+      <c r="B60" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="C60" s="33" t="s">
+      <c r="C60" s="37" t="s">
         <v>113</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -2399,9 +2402,9 @@
       </c>
     </row>
     <row r="61" spans="1:5" ht="15" customHeight="1">
-      <c r="A61" s="33"/>
-      <c r="B61" s="33"/>
-      <c r="C61" s="33"/>
+      <c r="A61" s="37"/>
+      <c r="B61" s="37"/>
+      <c r="C61" s="37"/>
       <c r="D61" s="1" t="s">
         <v>7</v>
       </c>
@@ -2410,72 +2413,72 @@
       </c>
     </row>
     <row r="62" spans="1:5" ht="15" customHeight="1">
-      <c r="A62" s="33"/>
+      <c r="A62" s="37"/>
       <c r="B62" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C62" s="36"/>
-      <c r="D62" s="36"/>
+      <c r="C62" s="38"/>
+      <c r="D62" s="38"/>
       <c r="E62" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="15" customHeight="1">
-      <c r="A63" s="33" t="s">
+      <c r="A63" s="37" t="s">
         <v>56</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C63" s="36" t="s">
+      <c r="C63" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="D63" s="36"/>
-      <c r="E63" s="36"/>
+      <c r="D63" s="38"/>
+      <c r="E63" s="38"/>
     </row>
     <row r="64" spans="1:5" ht="15" customHeight="1">
-      <c r="A64" s="33"/>
+      <c r="A64" s="37"/>
       <c r="B64" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C64" s="36"/>
-      <c r="D64" s="36"/>
+      <c r="C64" s="38"/>
+      <c r="D64" s="38"/>
       <c r="E64" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="15" customHeight="1">
-      <c r="A65" s="33" t="s">
+      <c r="A65" s="37" t="s">
         <v>65</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C65" s="36" t="s">
+      <c r="C65" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="D65" s="36"/>
-      <c r="E65" s="36"/>
+      <c r="D65" s="38"/>
+      <c r="E65" s="38"/>
     </row>
     <row r="66" spans="1:5" ht="15" customHeight="1">
-      <c r="A66" s="33"/>
+      <c r="A66" s="37"/>
       <c r="B66" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C66" s="36"/>
-      <c r="D66" s="36"/>
+      <c r="C66" s="38"/>
+      <c r="D66" s="38"/>
       <c r="E66" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="15" customHeight="1">
-      <c r="A67" s="32" t="s">
+      <c r="A67" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="B67" s="34" t="s">
+      <c r="B67" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="C67" s="34" t="s">
+      <c r="C67" s="35" t="s">
         <v>114</v>
       </c>
       <c r="D67" s="15" t="s">
@@ -2486,9 +2489,9 @@
       </c>
     </row>
     <row r="68" spans="1:5" ht="15" customHeight="1">
-      <c r="A68" s="32"/>
-      <c r="B68" s="34"/>
-      <c r="C68" s="34"/>
+      <c r="A68" s="36"/>
+      <c r="B68" s="35"/>
+      <c r="C68" s="35"/>
       <c r="D68" s="15" t="s">
         <v>7</v>
       </c>
@@ -2497,53 +2500,53 @@
       </c>
     </row>
     <row r="69" spans="1:5" ht="15" customHeight="1">
-      <c r="A69" s="32"/>
+      <c r="A69" s="36"/>
       <c r="B69" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C69" s="30"/>
-      <c r="D69" s="30"/>
+      <c r="C69" s="40"/>
+      <c r="D69" s="40"/>
       <c r="E69" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="15" customHeight="1">
-      <c r="A70" s="32"/>
+      <c r="A70" s="36"/>
       <c r="B70" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C70" s="30"/>
-      <c r="D70" s="30"/>
+      <c r="C70" s="40"/>
+      <c r="D70" s="40"/>
       <c r="E70" s="15" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15" customHeight="1">
-      <c r="A71" s="33" t="s">
+      <c r="A71" s="37" t="s">
         <v>45</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C71" s="35" t="s">
+      <c r="C71" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="D71" s="35"/>
-      <c r="E71" s="35"/>
+      <c r="D71" s="39"/>
+      <c r="E71" s="39"/>
     </row>
     <row r="72" spans="1:5" ht="15" customHeight="1">
-      <c r="A72" s="33"/>
+      <c r="A72" s="37"/>
       <c r="B72" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C72" s="35"/>
-      <c r="D72" s="35"/>
+      <c r="C72" s="39"/>
+      <c r="D72" s="39"/>
       <c r="E72" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="15" customHeight="1">
-      <c r="A73" s="31" t="s">
+      <c r="A73" s="42" t="s">
         <v>71</v>
       </c>
       <c r="B73" s="17" t="s">
@@ -2560,23 +2563,23 @@
       </c>
     </row>
     <row r="74" spans="1:5" ht="15" customHeight="1">
-      <c r="A74" s="31"/>
+      <c r="A74" s="42"/>
       <c r="B74" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C74" s="30"/>
-      <c r="D74" s="30"/>
+      <c r="C74" s="40"/>
+      <c r="D74" s="40"/>
       <c r="E74" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="15" customHeight="1">
-      <c r="A75" s="31"/>
+      <c r="A75" s="42"/>
       <c r="B75" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C75" s="30"/>
-      <c r="D75" s="30"/>
+      <c r="C75" s="40"/>
+      <c r="D75" s="40"/>
       <c r="E75" s="15" t="s">
         <v>74</v>
       </c>
@@ -2612,27 +2615,56 @@
     <row r="87" spans="3:4" s="2" customFormat="1" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="87">
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="A73:A75"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="A67:A70"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="C44:C45"/>
@@ -2649,56 +2681,27 @@
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="A73:A75"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="A67:A70"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:E48"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2742,13 +2745,13 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="49" t="s">
         <v>101</v>
       </c>
       <c r="D2" s="10" t="s">
@@ -2759,9 +2762,9 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="39"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
+      <c r="A3" s="48"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
       <c r="D3" s="10" t="s">
         <v>2</v>
       </c>
@@ -2770,9 +2773,9 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="39"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
+      <c r="A4" s="48"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
       <c r="D4" s="10" t="s">
         <v>4</v>
       </c>
@@ -2781,9 +2784,9 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="39"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
       <c r="D5" s="10" t="s">
         <v>5</v>
       </c>
@@ -2792,31 +2795,31 @@
       </c>
     </row>
     <row r="6" spans="1:5" hidden="1">
-      <c r="A6" s="39"/>
+      <c r="A6" s="48"/>
       <c r="B6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
       <c r="E6" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" hidden="1">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="43" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="42" t="s">
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="43" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="42"/>
+      <c r="A8" s="43"/>
       <c r="B8" s="8" t="s">
         <v>24</v>
       </c>
@@ -2824,28 +2827,28 @@
         <v>102</v>
       </c>
       <c r="D8" s="8"/>
-      <c r="E8" s="42"/>
+      <c r="E8" s="43"/>
     </row>
     <row r="9" spans="1:5" hidden="1">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="43" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
       <c r="E9" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:5" hidden="1">
-      <c r="A10" s="42"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
       <c r="E10" s="8" t="s">
         <v>28</v>
       </c>
@@ -2866,13 +2869,13 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="49" t="s">
         <v>104</v>
       </c>
       <c r="D12" s="10" t="s">
@@ -2883,9 +2886,9 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="39"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
+      <c r="A13" s="48"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
       <c r="D13" s="10" t="s">
         <v>5</v>
       </c>
@@ -2894,9 +2897,9 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="39"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="40"/>
+      <c r="A14" s="48"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="49"/>
       <c r="D14" s="10" t="s">
         <v>7</v>
       </c>
@@ -2911,62 +2914,62 @@
       <c r="B15" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
       <c r="E15" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:5" hidden="1">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="43" t="s">
         <v>39</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
       <c r="E16" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:5" hidden="1">
-      <c r="A17" s="42"/>
+      <c r="A17" s="43"/>
       <c r="B17" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
       <c r="E17" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="43" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="43" t="s">
+      <c r="C18" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
     </row>
     <row r="19" spans="1:5" hidden="1">
-      <c r="A19" s="42"/>
+      <c r="A19" s="43"/>
       <c r="B19" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
       <c r="E19" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="39" t="s">
+      <c r="A20" s="48" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="10" t="s">
@@ -2983,88 +2986,88 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1">
-      <c r="A21" s="39"/>
+      <c r="A21" s="48"/>
       <c r="B21" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
       <c r="E21" s="10" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:5" hidden="1">
-      <c r="A22" s="39"/>
+      <c r="A22" s="48"/>
       <c r="B22" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
       <c r="E22" s="10" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1">
-      <c r="A23" s="39"/>
+      <c r="A23" s="48"/>
       <c r="B23" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="49"/>
       <c r="E23" s="10" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1">
-      <c r="A24" s="39"/>
+      <c r="A24" s="48"/>
       <c r="B24" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
       <c r="E24" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:5" hidden="1">
-      <c r="A25" s="39"/>
+      <c r="A25" s="48"/>
       <c r="B25" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
       <c r="E25" s="10" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:5" hidden="1">
-      <c r="A26" s="39"/>
+      <c r="A26" s="48"/>
       <c r="B26" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
       <c r="E26" s="10" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:5" hidden="1">
-      <c r="A27" s="39"/>
+      <c r="A27" s="48"/>
       <c r="B27" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
       <c r="E27" s="10" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="39"/>
-      <c r="B28" s="40" t="s">
+      <c r="A28" s="48"/>
+      <c r="B28" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="40" t="s">
+      <c r="C28" s="49" t="s">
         <v>117</v>
       </c>
       <c r="D28" s="11" t="s">
@@ -3075,9 +3078,9 @@
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="39"/>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
+      <c r="A29" s="48"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
       <c r="D29" s="10" t="s">
         <v>7</v>
       </c>
@@ -3086,11 +3089,11 @@
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="39"/>
-      <c r="B30" s="40" t="s">
+      <c r="A30" s="48"/>
+      <c r="B30" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="40" t="s">
+      <c r="C30" s="49" t="s">
         <v>118</v>
       </c>
       <c r="D30" s="10" t="s">
@@ -3101,9 +3104,9 @@
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="39"/>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
+      <c r="A31" s="48"/>
+      <c r="B31" s="49"/>
+      <c r="C31" s="49"/>
       <c r="D31" s="10" t="s">
         <v>7</v>
       </c>
@@ -3112,11 +3115,11 @@
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="39"/>
-      <c r="B32" s="40" t="s">
+      <c r="A32" s="48"/>
+      <c r="B32" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="C32" s="49" t="s">
         <v>119</v>
       </c>
       <c r="D32" s="10" t="s">
@@ -3127,9 +3130,9 @@
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="39"/>
-      <c r="B33" s="40"/>
-      <c r="C33" s="40"/>
+      <c r="A33" s="48"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="49"/>
       <c r="D33" s="10" t="s">
         <v>7</v>
       </c>
@@ -3138,13 +3141,13 @@
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="42" t="s">
+      <c r="A34" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B34" s="42" t="s">
+      <c r="B34" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="42" t="s">
+      <c r="C34" s="43" t="s">
         <v>106</v>
       </c>
       <c r="D34" s="8" t="s">
@@ -3155,9 +3158,9 @@
       </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="42"/>
-      <c r="B35" s="42"/>
-      <c r="C35" s="42"/>
+      <c r="A35" s="43"/>
+      <c r="B35" s="43"/>
+      <c r="C35" s="43"/>
       <c r="D35" s="8" t="s">
         <v>7</v>
       </c>
@@ -3166,48 +3169,48 @@
       </c>
     </row>
     <row r="36" spans="1:5" hidden="1">
-      <c r="A36" s="42"/>
+      <c r="A36" s="43"/>
       <c r="B36" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="44"/>
-      <c r="D36" s="44"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="47"/>
       <c r="E36" s="8" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="42" t="s">
+      <c r="A37" s="43" t="s">
         <v>56</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="44" t="s">
+      <c r="C37" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="44"/>
-      <c r="E37" s="44"/>
+      <c r="D37" s="47"/>
+      <c r="E37" s="47"/>
     </row>
     <row r="38" spans="1:5" hidden="1">
-      <c r="A38" s="42"/>
+      <c r="A38" s="43"/>
       <c r="B38" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C38" s="44"/>
-      <c r="D38" s="44"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="47"/>
       <c r="E38" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="42" t="s">
+      <c r="A39" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="42" t="s">
+      <c r="B39" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="42" t="s">
+      <c r="C39" s="43" t="s">
         <v>107</v>
       </c>
       <c r="D39" s="8" t="s">
@@ -3218,9 +3221,9 @@
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="42"/>
-      <c r="B40" s="42"/>
-      <c r="C40" s="42"/>
+      <c r="A40" s="43"/>
+      <c r="B40" s="43"/>
+      <c r="C40" s="43"/>
       <c r="D40" s="8" t="s">
         <v>7</v>
       </c>
@@ -3229,13 +3232,13 @@
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="42" t="s">
+      <c r="A41" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="B41" s="42" t="s">
+      <c r="B41" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="C41" s="42" t="s">
+      <c r="C41" s="43" t="s">
         <v>120</v>
       </c>
       <c r="D41" s="8" t="s">
@@ -3246,9 +3249,9 @@
       </c>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="42"/>
-      <c r="B42" s="42"/>
-      <c r="C42" s="42"/>
+      <c r="A42" s="43"/>
+      <c r="B42" s="43"/>
+      <c r="C42" s="43"/>
       <c r="D42" s="8" t="s">
         <v>7</v>
       </c>
@@ -3257,24 +3260,24 @@
       </c>
     </row>
     <row r="43" spans="1:5" hidden="1">
-      <c r="A43" s="42"/>
+      <c r="A43" s="43"/>
       <c r="B43" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C43" s="44"/>
-      <c r="D43" s="44"/>
+      <c r="C43" s="47"/>
+      <c r="D43" s="47"/>
       <c r="E43" s="8" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="39" t="s">
+      <c r="A44" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="B44" s="40" t="s">
+      <c r="B44" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="40" t="s">
+      <c r="C44" s="49" t="s">
         <v>108</v>
       </c>
       <c r="D44" s="10" t="s">
@@ -3285,9 +3288,9 @@
       </c>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="39"/>
-      <c r="B45" s="40"/>
-      <c r="C45" s="40"/>
+      <c r="A45" s="48"/>
+      <c r="B45" s="49"/>
+      <c r="C45" s="49"/>
       <c r="D45" s="10" t="s">
         <v>7</v>
       </c>
@@ -3296,53 +3299,53 @@
       </c>
     </row>
     <row r="46" spans="1:5" hidden="1">
-      <c r="A46" s="39"/>
+      <c r="A46" s="48"/>
       <c r="B46" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C46" s="41"/>
-      <c r="D46" s="41"/>
+      <c r="C46" s="46"/>
+      <c r="D46" s="46"/>
       <c r="E46" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:5" hidden="1">
-      <c r="A47" s="39"/>
+      <c r="A47" s="48"/>
       <c r="B47" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C47" s="41"/>
-      <c r="D47" s="41"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="46"/>
       <c r="E47" s="10" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15" customHeight="1">
-      <c r="A48" s="42" t="s">
+      <c r="A48" s="43" t="s">
         <v>45</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C48" s="43" t="s">
+      <c r="C48" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="D48" s="43"/>
-      <c r="E48" s="43"/>
+      <c r="D48" s="44"/>
+      <c r="E48" s="44"/>
     </row>
     <row r="49" spans="1:5" hidden="1">
-      <c r="A49" s="42"/>
+      <c r="A49" s="43"/>
       <c r="B49" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="43"/>
-      <c r="D49" s="43"/>
+      <c r="C49" s="44"/>
+      <c r="D49" s="44"/>
       <c r="E49" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="30">
-      <c r="A50" s="39" t="s">
+      <c r="A50" s="48" t="s">
         <v>87</v>
       </c>
       <c r="B50" s="10" t="s">
@@ -3359,11 +3362,11 @@
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="39"/>
-      <c r="B51" s="40" t="s">
+      <c r="A51" s="48"/>
+      <c r="B51" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="C51" s="45" t="s">
+      <c r="C51" s="50" t="s">
         <v>110</v>
       </c>
       <c r="D51" s="12" t="s">
@@ -3374,9 +3377,9 @@
       </c>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="39"/>
-      <c r="B52" s="40"/>
-      <c r="C52" s="45"/>
+      <c r="A52" s="48"/>
+      <c r="B52" s="49"/>
+      <c r="C52" s="50"/>
       <c r="D52" s="12" t="s">
         <v>7</v>
       </c>
@@ -3385,7 +3388,7 @@
       </c>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="39" t="s">
+      <c r="A53" s="48" t="s">
         <v>8</v>
       </c>
       <c r="B53" s="10" t="s">
@@ -3402,33 +3405,33 @@
       </c>
     </row>
     <row r="54" spans="1:5" hidden="1">
-      <c r="A54" s="39"/>
+      <c r="A54" s="48"/>
       <c r="B54" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C54" s="41"/>
-      <c r="D54" s="41"/>
+      <c r="C54" s="46"/>
+      <c r="D54" s="46"/>
       <c r="E54" s="10" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:5" hidden="1">
-      <c r="A55" s="39"/>
+      <c r="A55" s="48"/>
       <c r="B55" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="41"/>
-      <c r="D55" s="41"/>
+      <c r="C55" s="46"/>
+      <c r="D55" s="46"/>
       <c r="E55" s="10" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="39"/>
-      <c r="B56" s="40" t="s">
+      <c r="A56" s="48"/>
+      <c r="B56" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="C56" s="40" t="s">
+      <c r="C56" s="49" t="s">
         <v>112</v>
       </c>
       <c r="D56" s="10" t="s">
@@ -3439,9 +3442,9 @@
       </c>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="39"/>
-      <c r="B57" s="40"/>
-      <c r="C57" s="40"/>
+      <c r="A57" s="48"/>
+      <c r="B57" s="49"/>
+      <c r="C57" s="49"/>
       <c r="D57" s="10" t="s">
         <v>7</v>
       </c>
@@ -3450,35 +3453,35 @@
       </c>
     </row>
     <row r="58" spans="1:5" hidden="1">
-      <c r="A58" s="39"/>
+      <c r="A58" s="48"/>
       <c r="B58" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C58" s="41"/>
-      <c r="D58" s="41"/>
+      <c r="C58" s="46"/>
+      <c r="D58" s="46"/>
       <c r="E58" s="10" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="59" spans="1:5" hidden="1">
-      <c r="A59" s="39"/>
+      <c r="A59" s="48"/>
       <c r="B59" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C59" s="41"/>
-      <c r="D59" s="41"/>
+      <c r="C59" s="46"/>
+      <c r="D59" s="46"/>
       <c r="E59" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="42" t="s">
+      <c r="A60" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B60" s="42" t="s">
+      <c r="B60" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="C60" s="42" t="s">
+      <c r="C60" s="43" t="s">
         <v>113</v>
       </c>
       <c r="D60" s="8" t="s">
@@ -3489,9 +3492,9 @@
       </c>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="42"/>
-      <c r="B61" s="42"/>
-      <c r="C61" s="42"/>
+      <c r="A61" s="43"/>
+      <c r="B61" s="43"/>
+      <c r="C61" s="43"/>
       <c r="D61" s="8" t="s">
         <v>7</v>
       </c>
@@ -3500,72 +3503,72 @@
       </c>
     </row>
     <row r="62" spans="1:5" hidden="1">
-      <c r="A62" s="42"/>
+      <c r="A62" s="43"/>
       <c r="B62" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C62" s="44"/>
-      <c r="D62" s="44"/>
+      <c r="C62" s="47"/>
+      <c r="D62" s="47"/>
       <c r="E62" s="8" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="42" t="s">
+      <c r="A63" s="43" t="s">
         <v>56</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C63" s="44" t="s">
+      <c r="C63" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="D63" s="44"/>
-      <c r="E63" s="44"/>
+      <c r="D63" s="47"/>
+      <c r="E63" s="47"/>
     </row>
     <row r="64" spans="1:5" hidden="1">
-      <c r="A64" s="42"/>
+      <c r="A64" s="43"/>
       <c r="B64" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C64" s="44"/>
-      <c r="D64" s="44"/>
+      <c r="C64" s="47"/>
+      <c r="D64" s="47"/>
       <c r="E64" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="42" t="s">
+      <c r="A65" s="43" t="s">
         <v>65</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C65" s="44" t="s">
+      <c r="C65" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="D65" s="44"/>
-      <c r="E65" s="44"/>
+      <c r="D65" s="47"/>
+      <c r="E65" s="47"/>
     </row>
     <row r="66" spans="1:5" hidden="1">
-      <c r="A66" s="42"/>
+      <c r="A66" s="43"/>
       <c r="B66" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C66" s="44"/>
-      <c r="D66" s="44"/>
+      <c r="C66" s="47"/>
+      <c r="D66" s="47"/>
       <c r="E66" s="8" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="39" t="s">
+      <c r="A67" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B67" s="40" t="s">
+      <c r="B67" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="C67" s="40" t="s">
+      <c r="C67" s="49" t="s">
         <v>114</v>
       </c>
       <c r="D67" s="10" t="s">
@@ -3576,9 +3579,9 @@
       </c>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="39"/>
-      <c r="B68" s="40"/>
-      <c r="C68" s="40"/>
+      <c r="A68" s="48"/>
+      <c r="B68" s="49"/>
+      <c r="C68" s="49"/>
       <c r="D68" s="10" t="s">
         <v>7</v>
       </c>
@@ -3587,53 +3590,53 @@
       </c>
     </row>
     <row r="69" spans="1:5" hidden="1">
-      <c r="A69" s="39"/>
+      <c r="A69" s="48"/>
       <c r="B69" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C69" s="41"/>
-      <c r="D69" s="41"/>
+      <c r="C69" s="46"/>
+      <c r="D69" s="46"/>
       <c r="E69" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="70" spans="1:5" hidden="1">
-      <c r="A70" s="39"/>
+      <c r="A70" s="48"/>
       <c r="B70" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C70" s="41"/>
-      <c r="D70" s="41"/>
+      <c r="C70" s="46"/>
+      <c r="D70" s="46"/>
       <c r="E70" s="10" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15" customHeight="1">
-      <c r="A71" s="42" t="s">
+      <c r="A71" s="43" t="s">
         <v>45</v>
       </c>
       <c r="B71" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C71" s="43" t="s">
+      <c r="C71" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="D71" s="43"/>
-      <c r="E71" s="43"/>
+      <c r="D71" s="44"/>
+      <c r="E71" s="44"/>
     </row>
     <row r="72" spans="1:5" hidden="1">
-      <c r="A72" s="42"/>
+      <c r="A72" s="43"/>
       <c r="B72" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C72" s="43"/>
-      <c r="D72" s="43"/>
+      <c r="C72" s="44"/>
+      <c r="D72" s="44"/>
       <c r="E72" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="46" t="s">
+      <c r="A73" s="45" t="s">
         <v>71</v>
       </c>
       <c r="B73" s="12" t="s">
@@ -3650,78 +3653,51 @@
       </c>
     </row>
     <row r="74" spans="1:5" hidden="1">
-      <c r="A74" s="46"/>
+      <c r="A74" s="45"/>
       <c r="B74" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C74" s="41"/>
-      <c r="D74" s="41"/>
+      <c r="C74" s="46"/>
+      <c r="D74" s="46"/>
       <c r="E74" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="75" spans="1:5" hidden="1">
-      <c r="A75" s="46"/>
+      <c r="A75" s="45"/>
       <c r="B75" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C75" s="41"/>
-      <c r="D75" s="41"/>
+      <c r="C75" s="46"/>
+      <c r="D75" s="46"/>
       <c r="E75" s="10" t="s">
         <v>74</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="87">
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="A73:A75"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="A67:A70"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:D19"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="C30:C31"/>
     <mergeCell ref="B32:B33"/>
@@ -3738,28 +3714,55 @@
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="C27:D27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="A67:A70"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="A73:A75"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
   </mergeCells>
   <conditionalFormatting sqref="A76:E100">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="0">
@@ -3780,14 +3783,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="55.83203125" customWidth="1"/>
     <col min="2" max="2" width="20.83203125" style="14" customWidth="1"/>
     <col min="3" max="4" width="55.83203125" style="24" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="51"/>
+    <col min="5" max="16384" width="10.83203125" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3808,13 +3813,13 @@
       <c r="A2" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="51" t="s">
         <v>121</v>
       </c>
       <c r="C2" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="30" t="s">
         <v>160</v>
       </c>
     </row>
@@ -3822,11 +3827,11 @@
       <c r="A3" s="27" t="s">
         <v>161</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="49" t="s">
+      <c r="B3" s="51"/>
+      <c r="C3" s="53" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="30" t="s">
         <v>166</v>
       </c>
     </row>
@@ -3834,29 +3839,29 @@
       <c r="A4" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="50" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="B4" s="51"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="30" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30">
       <c r="A5" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="50" t="s">
-        <v>167</v>
+      <c r="B5" s="51"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="30" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="375" customHeight="1">
       <c r="A6" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="B6" s="47"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="50" t="s">
+      <c r="B6" s="51"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="30" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3864,9 +3869,9 @@
       <c r="A7" s="27" t="s">
         <v>125</v>
       </c>
-      <c r="B7" s="47"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="50" t="s">
+      <c r="B7" s="51"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="30" t="s">
         <v>165</v>
       </c>
     </row>
@@ -3874,9 +3879,9 @@
       <c r="A8" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="50" t="s">
+      <c r="B8" s="51"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="30" t="s">
         <v>158</v>
       </c>
     </row>
@@ -3884,17 +3889,17 @@
       <c r="A9" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="50"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="30"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="B10" s="47"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="50" t="s">
+      <c r="B10" s="51"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="30" t="s">
         <v>165</v>
       </c>
     </row>
@@ -3902,9 +3907,9 @@
       <c r="A11" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="B11" s="47"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="50" t="s">
+      <c r="B11" s="51"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="30" t="s">
         <v>165</v>
       </c>
     </row>
@@ -3912,25 +3917,25 @@
       <c r="A12" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="B12" s="53" t="s">
+      <c r="B12" s="54" t="s">
         <v>131</v>
       </c>
-      <c r="C12" s="52" t="s">
+      <c r="C12" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="D12" s="50" t="s">
-        <v>166</v>
+      <c r="D12" s="30" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30">
       <c r="A13" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="B13" s="53"/>
+      <c r="B13" s="54"/>
       <c r="C13" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="D13" s="54" t="s">
+      <c r="D13" s="33" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3938,13 +3943,13 @@
       <c r="A14" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="52" t="s">
         <v>149</v>
       </c>
-      <c r="D14" s="50" t="s">
+      <c r="D14" s="30" t="s">
         <v>165</v>
       </c>
     </row>
@@ -3952,9 +3957,9 @@
       <c r="A15" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="B15" s="47"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="50" t="s">
+      <c r="B15" s="51"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="30" t="s">
         <v>165</v>
       </c>
     </row>
@@ -3962,9 +3967,9 @@
       <c r="A16" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="B16" s="47"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="50" t="s">
+      <c r="B16" s="51"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="30" t="s">
         <v>165</v>
       </c>
     </row>
@@ -3972,9 +3977,9 @@
       <c r="A17" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="B17" s="47"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="50" t="s">
+      <c r="B17" s="51"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="30" t="s">
         <v>165</v>
       </c>
     </row>
@@ -3982,11 +3987,11 @@
       <c r="A18" s="27" t="s">
         <v>140</v>
       </c>
-      <c r="B18" s="47"/>
+      <c r="B18" s="51"/>
       <c r="C18" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="D18" s="50" t="s">
+      <c r="D18" s="30" t="s">
         <v>165</v>
       </c>
     </row>
@@ -4000,7 +4005,7 @@
       <c r="C19" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="D19" s="50" t="s">
+      <c r="D19" s="30" t="s">
         <v>165</v>
       </c>
     </row>
@@ -4014,7 +4019,7 @@
       <c r="C20" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="D20" s="50" t="s">
+      <c r="D20" s="30" t="s">
         <v>165</v>
       </c>
     </row>
@@ -4026,7 +4031,7 @@
         <v>142</v>
       </c>
       <c r="C21" s="29"/>
-      <c r="D21" s="50"/>
+      <c r="D21" s="30"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="26" t="s">
@@ -4036,7 +4041,7 @@
         <v>144</v>
       </c>
       <c r="C22" s="29"/>
-      <c r="D22" s="50"/>
+      <c r="D22" s="30"/>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="20"/>

</xml_diff>

<commit_message>
update linkPage, add JobSeeker Service
</commit_message>
<xml_diff>
--- a/linksPage.xlsx
+++ b/linksPage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15680" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15900" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="linkTable" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="175">
   <si>
     <t>request</t>
   </si>
@@ -395,15 +395,6 @@
     <t>POST /account/restotrePassword</t>
   </si>
   <si>
-    <t>POST /jobSeeker/getProfile</t>
-  </si>
-  <si>
-    <t>POST /jobSeeker/delete</t>
-  </si>
-  <si>
-    <t>POST /jobSeeker/getResume</t>
-  </si>
-  <si>
     <t>POST /company/getProfile</t>
   </si>
   <si>
@@ -428,9 +419,6 @@
     <t>POST /jobSeeker/deactivateResume</t>
   </si>
   <si>
-    <t>POST /jobSeeker/verifyResume</t>
-  </si>
-  <si>
     <t>POST /jobSeeker/removeResume</t>
   </si>
   <si>
@@ -440,9 +428,6 @@
     <t>fieldsVisibilityDto</t>
   </si>
   <si>
-    <t>POST /jobSeeker/editProfile</t>
-  </si>
-  <si>
     <t>POST /jobSeeker/editResume</t>
   </si>
   <si>
@@ -488,20 +473,37 @@
     <t>{"login":"my@email.com","email":true,"firstName":true,"lastName":true,"birthDate":true,"phone":true,"location":true,"photo":true,"aboutMyself":true,"linkedin":true,"educations":true,"languages":true,"coursesAndCertificates":true,"recomendations":true,"experiences":true,"projects":true}</t>
   </si>
   <si>
-    <t>{"login":"my@email.com","downloadType":"doc","personData":{"firstName":"name","lastName":"surname","birthDate":"2017-12-06","phone":1234567,"location":"rehovot","photoUrl":"http://photoUrl"},"professionalData":{"aboutMySelf":"aboutMySelf","linkedinUrl":"http://linkedinUrl","educations":[{"nameUniversity":"university","nameSpeciality":"speciality","educationDegree":"master"}],"languages":[{"languageName":"english","languageLevel":"basic"}],"coursesAndCertificates":[{"nameOfCourse":"course","endDate":"2017-12-06"}],"recomendations":[{"firstName":"name","lastName":"surname","companyName":"company","position":"position","phone":1234567}],"experiences":[{"companyName":"company","position":"position","startDate":"2017-12-06","endDate":"2017-12-06","projects":[{"nameProject":"project","endDate":"2017-12-06","descriptionProject":"descriptionProject"}]}]},"fieldsVisibility":{"login":"my@Email.com","email":true,"firstName":true,"lastName":true,"birthDate":true,"phone":true,"location":true,"photo":true,"aboutMyself":true,"linkedin":true,"educations":true,"languages":true,"coursesAndCertificates":true,"recomendations":true,"experiences":true,"projects":true}}</t>
-  </si>
-  <si>
     <t>{"login":"my@email.com"}</t>
   </si>
   <si>
     <t>{"login":"my@email.com","password":"1234567"}</t>
   </si>
   <si>
-    <t>{"login":"my@email.com","yearsInWork":1,"skillsType":["java"],"companyName":["myCompany1"],"verification":{"date":"2017-12-06","verificationStatus":"yes"},"cvType":"backEnd","dateOfEnable":"2017-12-06","enable":true}</t>
-  </si>
-  <si>
-    <t>{"login":"my@Email.com","downloadType":"doc","curriculumVitae":[{"yearsInWork":1,"skillsType":["java"],"companyName":["myCompany1"],"verification":{"date":"2017-12-06","verificationStatus":"yes"},"cvType":"backEnd","dateOfEnable":"2017-12-06","enable":true}],"personData":{"firstName":"name","lastName":"surname","birthDate":"2017-12-07","phone":1234567,"location":"rehovot","photoUrl":"http://photoUrl"},"professionalData":{"aboutMySelf":"aboutMySelf","linkedinUrl":"http://linkedinUrl","educations":[{"nameUniversity":"university","nameSpeciality":"speciality","educationDegree":"master"}],"languages":[{"languageName":"english","languageLevel":"basic"}],"coursesAndCertificates":[{"nameOfCourse":"course","endDate":"2017-12-06"}],"recomendations":[{"firstName":"name","lastName":"surname","companyName":"company","position":"position","phone":1234567}],"experiences":[{"companyName":"company","position":"position","startDate":"2017-12-06","endDate":"2017-12-06","projects":[{"nameProject":"project","endDate":"2017-12-06","descriptionProject":"descriptionProject"}]}]},
-"fieldsVisibility":{"login":"my@Email.com","email":true,"firstName":true,"lastName":true,"birthDate":true,"phone":true,"location":true,"photo":true,"aboutMyself":true,"linkedin":true,"educations":true,"languages":true,"coursesAndCertificates":true,"recomendations":true,"experiences":true,"projects":true}}</t>
+    <t>POST /account/isExist</t>
+  </si>
+  <si>
+    <t>POST /account/checkQuestion</t>
+  </si>
+  <si>
+    <t>{"login":"my@email.com","typeQuestion":"question1","question":"answerToQuestion"}</t>
+  </si>
+  <si>
+    <t>"notActivated" / "wrongCredentials" / "noSendEmail" / "false"</t>
+  </si>
+  <si>
+    <t>"ok" / "false"</t>
+  </si>
+  <si>
+    <t>"ok" / "false" / "wrongRequest"</t>
+  </si>
+  <si>
+    <t>"ok" / "noSendEmail / "wrongRequest" / "wrongCredentials"</t>
+  </si>
+  <si>
+    <t>"ok" / "false" / "wrongRequest" / "noSendEmail" / "wrongCredentials"</t>
+  </si>
+  <si>
+    <t>"ok" / "false" / "wrongRequest" / "wrongCredentials"</t>
   </si>
   <si>
     <r>
@@ -513,42 +515,54 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> "remove" / "wrongRequest" / </t>
+      <t xml:space="preserve"> "remove" / "wrongRequest"</t>
     </r>
   </si>
   <si>
-    <t>POST /account/isExist</t>
-  </si>
-  <si>
-    <t>POST /account/checkQuestion</t>
-  </si>
-  <si>
-    <t>{"login":"my@email.com","typeQuestion":"question1","question":"answerToQuestion"}</t>
-  </si>
-  <si>
-    <t>"notActivated" / "wrongCredentials" / "noSendEmail" / "false"</t>
-  </si>
-  <si>
-    <t>"ok" / "false"</t>
-  </si>
-  <si>
-    <t>"ok" / "false" / "wrongRequest"</t>
-  </si>
-  <si>
-    <t>"ok" / "noSendEmail / "wrongRequest" / "wrongCredentials"</t>
-  </si>
-  <si>
-    <t>"ok" / "false" / "wrongRequest" / "noSendEmail" / "wrongCredentials"</t>
-  </si>
-  <si>
-    <t>"ok" / "false" / "wrongRequest" / "wrongCredentials"</t>
+    <t>POST /jobSeeker/getResumes</t>
+  </si>
+  <si>
+    <t>POST /jobSeeker/verifyResume/inProcess</t>
+  </si>
+  <si>
+    <t>POST /jobSeeker/createProfile</t>
+  </si>
+  <si>
+    <t>POST /jobSeeker/readProfile</t>
+  </si>
+  <si>
+    <t>POST /jobSeeker/deleteProfile</t>
+  </si>
+  <si>
+    <t>POST /jobSeeker/updateProfile</t>
+  </si>
+  <si>
+    <t>{"login":"my@Email.com","downloadType":"doc","personData":{"firstName":"name","lastName":"surname","birthDate":"2017-12-07","phone":1234567,"location":"rehovot","photoUrl":"http://photoUrl"},"professionalData":{"aboutMySelf":"aboutMySelf","linkedinUrl":"http://linkedinUrl","educations":[{"nameUniversity":"university","nameSpeciality":"speciality","educationDegree":"master","startDate":"2017-12-06","endDate":"2017-12-06"}],"languages":[{"languageName":"english","languageLevel":"basic"}],"coursesAndCertificates":[{"nameOfCourse":"course","endDate":"2017-12-06"}],"recomendations":[{"firstName":"name","lastName":"surname","companyName":"company","position":"position","phone":1234567}],"experiences":[{"companyName":"company","position":"position","startDate":"2017-12-06","endDate":"2017-12-06","projects":[{"nameProject":"project","endDate":"2017-12-06","descriptionProject":"descriptionProject"}]}]}}</t>
+  </si>
+  <si>
+    <t>"ok" / "wrongRequest" / "exist" / "removed"</t>
+  </si>
+  <si>
+    <t>"ok" / "noFound" / "removed"</t>
+  </si>
+  <si>
+    <t>{"login":"my@Email.com","downloadType":"doc","personData":{"firstName":"name","lastName":"surname","phone":12345671,"location":"rehovot","photoUrl":"http://photoUrl"},"professionalData":{"aboutMySelf":"aboutMySelf","linkedinUrl":"http://linkedinUrl","educations":[{"nameUniversity":"university","nameSpeciality":"speciality","educationDegree":"master","startDate":"2017-12-06","endDate":"2017-12-06"}],"languages":[{"languageName":"english","languageLevel":"basic"}],"coursesAndCertificates":[{"nameOfCourse":"course","endDate":"2017-12-06"}],"recomendations":[{"firstName":"name","lastName":"surname","companyName":"company","position":"position","phone":1234567}],"experiences":[{"companyName":"company1","position":"position1","startDate":"2011-12-06","endDate":"2011-12-06","projects":[{"nameProject":"project1","endDate":"2011-12-06","descriptionProject":"descriptionProject1"}]}]}}</t>
+  </si>
+  <si>
+    <t>"noFound" / "remove" / "false" {"login":"my@Email.com","downloadType":"doc","curriculumVitae":[{"login":"my@Email.com","yearsInWork":1,"skillsType":["java"],"companyName":["myCompany1"],"verification":{"date":"2017-12-06","verificationStatus":"yes"},"cvType":"backEnd","dateOfEnable":"2017-12-06","enable":true,"minSalary":1}],"personData":{"firstName":"name","lastName":"surname","birthDate":"2017-12-07","phone":1234567,"location":"rehovot","photoUrl":"http://photoUrl"},"professionalData":{"aboutMySelf":"aboutMySelf","linkedinUrl":"http://linkedinUrl","educations":[{"nameUniversity":"university","nameSpeciality":"speciality","educationDegree":"master","startDate":"2017-12-06","endDate":"2017-12-06"}],"languages":[{"languageName":"english","languageLevel":"basic"}],"coursesAndCertificates":[{"nameOfCourse":"course","endDate":"2017-12-06"}],"recomendations":[{"firstName":"name","lastName":"surname","companyName":"company","position":"position","phone":1234567}],"experiences":[{"companyName":"company","position":"position","startDate":"2017-12-06","endDate":"2017-12-06","projects":[{"nameProject":"project","endDate":"2017-12-06","descriptionProject":"descriptionProject"}]}]},"fieldsVisibility":{"login":"my@Email.com","email":true,"firstName":true,"lastName":true,"birthDate":true,"phone":true,"location":true,"photo":true,"aboutMyself":true,"linkedin":true,"educations":true,"languages":true,"coursesAndCertificates":true,"recomendations":true,"experiences":true,"projects":true}}</t>
+  </si>
+  <si>
+    <t>"ok" / "noFound"</t>
+  </si>
+  <si>
+    <t>POST /jobSeeker/restoreProfile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -603,8 +617,15 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -629,6 +650,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -639,7 +666,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="237">
+  <cellStyleXfs count="249">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -877,8 +904,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -944,63 +983,66 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1008,38 +1050,59 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="237">
+  <cellStyles count="249">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="5" builtinId="8" hidden="1"/>
@@ -1158,6 +1221,12 @@
     <cellStyle name="Гиперссылка" xfId="231" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="233" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="247" builtinId="8" hidden="1"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="4" builtinId="9" hidden="1"/>
@@ -1277,6 +1346,12 @@
     <cellStyle name="Просмотренная гиперссылка" xfId="232" builtinId="9" hidden="1"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="234" builtinId="9" hidden="1"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="248" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1625,8 +1700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:C14"/>
+    <sheetView showRuler="0" topLeftCell="B35" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -1656,14 +1731,14 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="35" t="s">
-        <v>147</v>
+      <c r="C2" s="36" t="s">
+        <v>142</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>3</v>
@@ -1673,9 +1748,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="36"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
       <c r="D3" s="15" t="s">
         <v>2</v>
       </c>
@@ -1684,9 +1759,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1">
-      <c r="A4" s="36"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
       <c r="D4" s="15" t="s">
         <v>4</v>
       </c>
@@ -1695,9 +1770,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1">
-      <c r="A5" s="36"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
       <c r="D5" s="15" t="s">
         <v>5</v>
       </c>
@@ -1706,41 +1781,41 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1">
-      <c r="A6" s="36"/>
+      <c r="A6" s="34"/>
       <c r="B6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
       <c r="E6" s="15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="35" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="37" t="s">
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="35" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
-      <c r="A8" s="37"/>
+      <c r="A8" s="35"/>
       <c r="B8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="37"/>
+      <c r="E8" s="35"/>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="35" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1753,7 +1828,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1">
-      <c r="A10" s="37"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
@@ -1779,13 +1854,13 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="36" t="s">
         <v>104</v>
       </c>
       <c r="D12" s="15" t="s">
@@ -1796,9 +1871,9 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1">
-      <c r="A13" s="36"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
+      <c r="A13" s="34"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
       <c r="D13" s="15" t="s">
         <v>5</v>
       </c>
@@ -1807,9 +1882,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1">
-      <c r="A14" s="36"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="35"/>
+      <c r="A14" s="34"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="15" t="s">
         <v>7</v>
       </c>
@@ -1831,7 +1906,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="35" t="s">
         <v>39</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1844,7 +1919,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1">
-      <c r="A17" s="37"/>
+      <c r="A17" s="35"/>
       <c r="B17" s="1" t="s">
         <v>41</v>
       </c>
@@ -1855,20 +1930,20 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="35" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1">
-      <c r="A19" s="37"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="1" t="s">
         <v>41</v>
       </c>
@@ -1879,7 +1954,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="34" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="15" t="s">
@@ -1896,88 +1971,88 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1">
-      <c r="A21" s="36"/>
+      <c r="A21" s="34"/>
       <c r="B21" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
       <c r="E21" s="15" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1">
-      <c r="A22" s="36"/>
+      <c r="A22" s="34"/>
       <c r="B22" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
       <c r="E22" s="15" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1">
-      <c r="A23" s="36"/>
+      <c r="A23" s="34"/>
       <c r="B23" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
       <c r="E23" s="15" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1">
-      <c r="A24" s="36"/>
+      <c r="A24" s="34"/>
       <c r="B24" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
       <c r="E24" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1">
-      <c r="A25" s="36"/>
+      <c r="A25" s="34"/>
       <c r="B25" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
       <c r="E25" s="15" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1">
-      <c r="A26" s="36"/>
+      <c r="A26" s="34"/>
       <c r="B26" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
       <c r="E26" s="15" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1">
-      <c r="A27" s="36"/>
+      <c r="A27" s="34"/>
       <c r="B27" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
       <c r="E27" s="15" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" customHeight="1">
-      <c r="A28" s="36"/>
-      <c r="B28" s="35" t="s">
+      <c r="A28" s="34"/>
+      <c r="B28" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="35" t="s">
+      <c r="C28" s="36" t="s">
         <v>117</v>
       </c>
       <c r="D28" s="16" t="s">
@@ -1988,9 +2063,9 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" customHeight="1">
-      <c r="A29" s="36"/>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
+      <c r="A29" s="34"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
       <c r="D29" s="15" t="s">
         <v>7</v>
       </c>
@@ -1999,11 +2074,11 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" customHeight="1">
-      <c r="A30" s="36"/>
-      <c r="B30" s="35" t="s">
+      <c r="A30" s="34"/>
+      <c r="B30" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="35" t="s">
+      <c r="C30" s="36" t="s">
         <v>118</v>
       </c>
       <c r="D30" s="15" t="s">
@@ -2014,9 +2089,9 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="15" customHeight="1">
-      <c r="A31" s="36"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="35"/>
+      <c r="A31" s="34"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="36"/>
       <c r="D31" s="15" t="s">
         <v>7</v>
       </c>
@@ -2025,11 +2100,11 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" customHeight="1">
-      <c r="A32" s="36"/>
-      <c r="B32" s="35" t="s">
+      <c r="A32" s="34"/>
+      <c r="B32" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="35" t="s">
+      <c r="C32" s="36" t="s">
         <v>119</v>
       </c>
       <c r="D32" s="15" t="s">
@@ -2040,9 +2115,9 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" customHeight="1">
-      <c r="A33" s="36"/>
-      <c r="B33" s="35"/>
-      <c r="C33" s="35"/>
+      <c r="A33" s="34"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="36"/>
       <c r="D33" s="15" t="s">
         <v>7</v>
       </c>
@@ -2051,13 +2126,13 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" customHeight="1">
-      <c r="A34" s="37" t="s">
+      <c r="A34" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="B34" s="37" t="s">
+      <c r="B34" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="37" t="s">
+      <c r="C34" s="35" t="s">
         <v>106</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -2068,9 +2143,9 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" customHeight="1">
-      <c r="A35" s="37"/>
-      <c r="B35" s="37"/>
-      <c r="C35" s="37"/>
+      <c r="A35" s="35"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
       <c r="D35" s="1" t="s">
         <v>7</v>
       </c>
@@ -2079,7 +2154,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" customHeight="1">
-      <c r="A36" s="37"/>
+      <c r="A36" s="35"/>
       <c r="B36" s="1" t="s">
         <v>53</v>
       </c>
@@ -2090,7 +2165,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" customHeight="1">
-      <c r="A37" s="37" t="s">
+      <c r="A37" s="35" t="s">
         <v>56</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -2103,7 +2178,7 @@
       <c r="E37" s="38"/>
     </row>
     <row r="38" spans="1:5" ht="15" customHeight="1">
-      <c r="A38" s="37"/>
+      <c r="A38" s="35"/>
       <c r="B38" s="1" t="s">
         <v>58</v>
       </c>
@@ -2114,13 +2189,13 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="15" customHeight="1">
-      <c r="A39" s="37" t="s">
+      <c r="A39" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="37" t="s">
+      <c r="B39" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="37" t="s">
+      <c r="C39" s="35" t="s">
         <v>107</v>
       </c>
       <c r="D39" s="1" t="s">
@@ -2131,9 +2206,9 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="15" customHeight="1">
-      <c r="A40" s="37"/>
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
+      <c r="A40" s="35"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="35"/>
       <c r="D40" s="1" t="s">
         <v>7</v>
       </c>
@@ -2142,13 +2217,13 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="15" customHeight="1">
-      <c r="A41" s="37" t="s">
+      <c r="A41" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="B41" s="37" t="s">
+      <c r="B41" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="C41" s="37" t="s">
+      <c r="C41" s="35" t="s">
         <v>120</v>
       </c>
       <c r="D41" s="1" t="s">
@@ -2159,9 +2234,9 @@
       </c>
     </row>
     <row r="42" spans="1:5" ht="15" customHeight="1">
-      <c r="A42" s="37"/>
-      <c r="B42" s="37"/>
-      <c r="C42" s="37"/>
+      <c r="A42" s="35"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="35"/>
       <c r="D42" s="1" t="s">
         <v>7</v>
       </c>
@@ -2170,7 +2245,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" customHeight="1">
-      <c r="A43" s="37"/>
+      <c r="A43" s="35"/>
       <c r="B43" s="1" t="s">
         <v>53</v>
       </c>
@@ -2181,13 +2256,13 @@
       </c>
     </row>
     <row r="44" spans="1:5" ht="15" customHeight="1">
-      <c r="A44" s="36" t="s">
+      <c r="A44" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B44" s="35" t="s">
+      <c r="B44" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="35" t="s">
+      <c r="C44" s="36" t="s">
         <v>108</v>
       </c>
       <c r="D44" s="15" t="s">
@@ -2198,9 +2273,9 @@
       </c>
     </row>
     <row r="45" spans="1:5" ht="15" customHeight="1">
-      <c r="A45" s="36"/>
-      <c r="B45" s="35"/>
-      <c r="C45" s="35"/>
+      <c r="A45" s="34"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="36"/>
       <c r="D45" s="15" t="s">
         <v>7</v>
       </c>
@@ -2209,53 +2284,53 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="15" customHeight="1">
-      <c r="A46" s="36"/>
+      <c r="A46" s="34"/>
       <c r="B46" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C46" s="40"/>
-      <c r="D46" s="40"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
       <c r="E46" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15" customHeight="1">
-      <c r="A47" s="36"/>
+      <c r="A47" s="34"/>
       <c r="B47" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C47" s="40"/>
-      <c r="D47" s="40"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
       <c r="E47" s="15" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15" customHeight="1">
-      <c r="A48" s="37" t="s">
+      <c r="A48" s="35" t="s">
         <v>45</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C48" s="39" t="s">
+      <c r="C48" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="D48" s="39"/>
-      <c r="E48" s="39"/>
+      <c r="D48" s="37"/>
+      <c r="E48" s="37"/>
     </row>
     <row r="49" spans="1:5" ht="15" customHeight="1">
-      <c r="A49" s="37"/>
+      <c r="A49" s="35"/>
       <c r="B49" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="39"/>
-      <c r="D49" s="39"/>
+      <c r="C49" s="37"/>
+      <c r="D49" s="37"/>
       <c r="E49" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="30" customHeight="1">
-      <c r="A50" s="36" t="s">
+      <c r="A50" s="34" t="s">
         <v>87</v>
       </c>
       <c r="B50" s="15" t="s">
@@ -2272,11 +2347,11 @@
       </c>
     </row>
     <row r="51" spans="1:5" ht="15" customHeight="1">
-      <c r="A51" s="36"/>
-      <c r="B51" s="35" t="s">
+      <c r="A51" s="34"/>
+      <c r="B51" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="C51" s="34" t="s">
+      <c r="C51" s="40" t="s">
         <v>110</v>
       </c>
       <c r="D51" s="17" t="s">
@@ -2287,9 +2362,9 @@
       </c>
     </row>
     <row r="52" spans="1:5" ht="15" customHeight="1">
-      <c r="A52" s="36"/>
-      <c r="B52" s="35"/>
-      <c r="C52" s="34"/>
+      <c r="A52" s="34"/>
+      <c r="B52" s="36"/>
+      <c r="C52" s="40"/>
       <c r="D52" s="17" t="s">
         <v>7</v>
       </c>
@@ -2298,7 +2373,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" ht="15" customHeight="1">
-      <c r="A53" s="36" t="s">
+      <c r="A53" s="34" t="s">
         <v>8</v>
       </c>
       <c r="B53" s="15" t="s">
@@ -2308,40 +2383,40 @@
         <v>111</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E53" s="15" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15" customHeight="1">
-      <c r="A54" s="36"/>
+      <c r="A54" s="34"/>
       <c r="B54" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C54" s="40"/>
-      <c r="D54" s="40"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="32"/>
       <c r="E54" s="15" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15" customHeight="1">
-      <c r="A55" s="36"/>
+      <c r="A55" s="34"/>
       <c r="B55" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="40"/>
-      <c r="D55" s="40"/>
+      <c r="C55" s="32"/>
+      <c r="D55" s="32"/>
       <c r="E55" s="15" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15" customHeight="1">
-      <c r="A56" s="36"/>
-      <c r="B56" s="35" t="s">
+      <c r="A56" s="34"/>
+      <c r="B56" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="C56" s="35" t="s">
+      <c r="C56" s="36" t="s">
         <v>112</v>
       </c>
       <c r="D56" s="15" t="s">
@@ -2352,9 +2427,9 @@
       </c>
     </row>
     <row r="57" spans="1:5" ht="15" customHeight="1">
-      <c r="A57" s="36"/>
-      <c r="B57" s="35"/>
-      <c r="C57" s="35"/>
+      <c r="A57" s="34"/>
+      <c r="B57" s="36"/>
+      <c r="C57" s="36"/>
       <c r="D57" s="15" t="s">
         <v>7</v>
       </c>
@@ -2363,35 +2438,35 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="15" customHeight="1">
-      <c r="A58" s="36"/>
+      <c r="A58" s="34"/>
       <c r="B58" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C58" s="40"/>
-      <c r="D58" s="40"/>
+      <c r="C58" s="32"/>
+      <c r="D58" s="32"/>
       <c r="E58" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15" customHeight="1">
-      <c r="A59" s="36"/>
+      <c r="A59" s="34"/>
       <c r="B59" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C59" s="40"/>
-      <c r="D59" s="40"/>
+      <c r="C59" s="32"/>
+      <c r="D59" s="32"/>
       <c r="E59" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15" customHeight="1">
-      <c r="A60" s="37" t="s">
+      <c r="A60" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="B60" s="37" t="s">
+      <c r="B60" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="C60" s="37" t="s">
+      <c r="C60" s="35" t="s">
         <v>113</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -2402,9 +2477,9 @@
       </c>
     </row>
     <row r="61" spans="1:5" ht="15" customHeight="1">
-      <c r="A61" s="37"/>
-      <c r="B61" s="37"/>
-      <c r="C61" s="37"/>
+      <c r="A61" s="35"/>
+      <c r="B61" s="35"/>
+      <c r="C61" s="35"/>
       <c r="D61" s="1" t="s">
         <v>7</v>
       </c>
@@ -2413,7 +2488,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" ht="15" customHeight="1">
-      <c r="A62" s="37"/>
+      <c r="A62" s="35"/>
       <c r="B62" s="1" t="s">
         <v>53</v>
       </c>
@@ -2424,7 +2499,7 @@
       </c>
     </row>
     <row r="63" spans="1:5" ht="15" customHeight="1">
-      <c r="A63" s="37" t="s">
+      <c r="A63" s="35" t="s">
         <v>56</v>
       </c>
       <c r="B63" s="1" t="s">
@@ -2437,7 +2512,7 @@
       <c r="E63" s="38"/>
     </row>
     <row r="64" spans="1:5" ht="15" customHeight="1">
-      <c r="A64" s="37"/>
+      <c r="A64" s="35"/>
       <c r="B64" s="1" t="s">
         <v>58</v>
       </c>
@@ -2448,7 +2523,7 @@
       </c>
     </row>
     <row r="65" spans="1:5" ht="15" customHeight="1">
-      <c r="A65" s="37" t="s">
+      <c r="A65" s="35" t="s">
         <v>65</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -2461,7 +2536,7 @@
       <c r="E65" s="38"/>
     </row>
     <row r="66" spans="1:5" ht="15" customHeight="1">
-      <c r="A66" s="37"/>
+      <c r="A66" s="35"/>
       <c r="B66" s="1" t="s">
         <v>67</v>
       </c>
@@ -2472,13 +2547,13 @@
       </c>
     </row>
     <row r="67" spans="1:5" ht="15" customHeight="1">
-      <c r="A67" s="36" t="s">
+      <c r="A67" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="B67" s="35" t="s">
+      <c r="B67" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="C67" s="35" t="s">
+      <c r="C67" s="36" t="s">
         <v>114</v>
       </c>
       <c r="D67" s="15" t="s">
@@ -2489,9 +2564,9 @@
       </c>
     </row>
     <row r="68" spans="1:5" ht="15" customHeight="1">
-      <c r="A68" s="36"/>
-      <c r="B68" s="35"/>
-      <c r="C68" s="35"/>
+      <c r="A68" s="34"/>
+      <c r="B68" s="36"/>
+      <c r="C68" s="36"/>
       <c r="D68" s="15" t="s">
         <v>7</v>
       </c>
@@ -2500,53 +2575,53 @@
       </c>
     </row>
     <row r="69" spans="1:5" ht="15" customHeight="1">
-      <c r="A69" s="36"/>
+      <c r="A69" s="34"/>
       <c r="B69" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C69" s="40"/>
-      <c r="D69" s="40"/>
+      <c r="C69" s="32"/>
+      <c r="D69" s="32"/>
       <c r="E69" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="15" customHeight="1">
-      <c r="A70" s="36"/>
+      <c r="A70" s="34"/>
       <c r="B70" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C70" s="40"/>
-      <c r="D70" s="40"/>
+      <c r="C70" s="32"/>
+      <c r="D70" s="32"/>
       <c r="E70" s="15" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15" customHeight="1">
-      <c r="A71" s="37" t="s">
+      <c r="A71" s="35" t="s">
         <v>45</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C71" s="39" t="s">
+      <c r="C71" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="D71" s="39"/>
-      <c r="E71" s="39"/>
+      <c r="D71" s="37"/>
+      <c r="E71" s="37"/>
     </row>
     <row r="72" spans="1:5" ht="15" customHeight="1">
-      <c r="A72" s="37"/>
+      <c r="A72" s="35"/>
       <c r="B72" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C72" s="39"/>
-      <c r="D72" s="39"/>
+      <c r="C72" s="37"/>
+      <c r="D72" s="37"/>
       <c r="E72" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="15" customHeight="1">
-      <c r="A73" s="42" t="s">
+      <c r="A73" s="33" t="s">
         <v>71</v>
       </c>
       <c r="B73" s="17" t="s">
@@ -2563,23 +2638,23 @@
       </c>
     </row>
     <row r="74" spans="1:5" ht="15" customHeight="1">
-      <c r="A74" s="42"/>
+      <c r="A74" s="33"/>
       <c r="B74" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C74" s="40"/>
-      <c r="D74" s="40"/>
+      <c r="C74" s="32"/>
+      <c r="D74" s="32"/>
       <c r="E74" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="15" customHeight="1">
-      <c r="A75" s="42"/>
+      <c r="A75" s="33"/>
       <c r="B75" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C75" s="40"/>
-      <c r="D75" s="40"/>
+      <c r="C75" s="32"/>
+      <c r="D75" s="32"/>
       <c r="E75" s="15" t="s">
         <v>74</v>
       </c>
@@ -2615,17 +2690,66 @@
     <row r="87" spans="3:4" s="2" customFormat="1" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="87">
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="A73:A75"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="A67:A70"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="A20:A33"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:C40"/>
     <mergeCell ref="C65:E65"/>
     <mergeCell ref="C66:D66"/>
     <mergeCell ref="A65:A66"/>
@@ -2642,66 +2766,17 @@
     <mergeCell ref="C64:D64"/>
     <mergeCell ref="C63:E63"/>
     <mergeCell ref="C56:C57"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="A20:A33"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="A73:A75"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="A67:A70"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C70:D70"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2745,13 +2820,13 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="42" t="s">
         <v>101</v>
       </c>
       <c r="D2" s="10" t="s">
@@ -2762,9 +2837,9 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="48"/>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
       <c r="D3" s="10" t="s">
         <v>2</v>
       </c>
@@ -2773,9 +2848,9 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="48"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
       <c r="D4" s="10" t="s">
         <v>4</v>
       </c>
@@ -2784,9 +2859,9 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="48"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
+      <c r="A5" s="41"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
       <c r="D5" s="10" t="s">
         <v>5</v>
       </c>
@@ -2795,31 +2870,31 @@
       </c>
     </row>
     <row r="6" spans="1:5" hidden="1">
-      <c r="A6" s="48"/>
+      <c r="A6" s="41"/>
       <c r="B6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
       <c r="E6" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" hidden="1">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="44" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="43" t="s">
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="44" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="43"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="8" t="s">
         <v>24</v>
       </c>
@@ -2827,28 +2902,28 @@
         <v>102</v>
       </c>
       <c r="D8" s="8"/>
-      <c r="E8" s="43"/>
+      <c r="E8" s="44"/>
     </row>
     <row r="9" spans="1:5" hidden="1">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="44" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
       <c r="E9" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:5" hidden="1">
-      <c r="A10" s="43"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
       <c r="E10" s="8" t="s">
         <v>28</v>
       </c>
@@ -2869,13 +2944,13 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="49" t="s">
+      <c r="C12" s="42" t="s">
         <v>104</v>
       </c>
       <c r="D12" s="10" t="s">
@@ -2886,9 +2961,9 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="48"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="49"/>
+      <c r="A13" s="41"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
       <c r="D13" s="10" t="s">
         <v>5</v>
       </c>
@@ -2897,9 +2972,9 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="48"/>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
       <c r="D14" s="10" t="s">
         <v>7</v>
       </c>
@@ -2914,62 +2989,62 @@
       <c r="B15" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="47"/>
-      <c r="D15" s="47"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46"/>
       <c r="E15" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:5" hidden="1">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="44" t="s">
         <v>39</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="47"/>
-      <c r="D16" s="47"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
       <c r="E16" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:5" hidden="1">
-      <c r="A17" s="43"/>
+      <c r="A17" s="44"/>
       <c r="B17" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
       <c r="E17" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="44" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="44" t="s">
+      <c r="C18" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="44"/>
-      <c r="E18" s="44"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
     </row>
     <row r="19" spans="1:5" hidden="1">
-      <c r="A19" s="43"/>
+      <c r="A19" s="44"/>
       <c r="B19" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="46"/>
       <c r="E19" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="48" t="s">
+      <c r="A20" s="41" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="10" t="s">
@@ -2986,88 +3061,88 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1">
-      <c r="A21" s="48"/>
+      <c r="A21" s="41"/>
       <c r="B21" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
       <c r="E21" s="10" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:5" hidden="1">
-      <c r="A22" s="48"/>
+      <c r="A22" s="41"/>
       <c r="B22" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
       <c r="E22" s="10" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1">
-      <c r="A23" s="48"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
       <c r="E23" s="10" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1">
-      <c r="A24" s="48"/>
+      <c r="A24" s="41"/>
       <c r="B24" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
       <c r="E24" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:5" hidden="1">
-      <c r="A25" s="48"/>
+      <c r="A25" s="41"/>
       <c r="B25" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
       <c r="E25" s="10" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:5" hidden="1">
-      <c r="A26" s="48"/>
+      <c r="A26" s="41"/>
       <c r="B26" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
       <c r="E26" s="10" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:5" hidden="1">
-      <c r="A27" s="48"/>
+      <c r="A27" s="41"/>
       <c r="B27" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="46"/>
-      <c r="D27" s="46"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
       <c r="E27" s="10" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="48"/>
-      <c r="B28" s="49" t="s">
+      <c r="A28" s="41"/>
+      <c r="B28" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="49" t="s">
+      <c r="C28" s="42" t="s">
         <v>117</v>
       </c>
       <c r="D28" s="11" t="s">
@@ -3078,9 +3153,9 @@
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="48"/>
-      <c r="B29" s="49"/>
-      <c r="C29" s="49"/>
+      <c r="A29" s="41"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="42"/>
       <c r="D29" s="10" t="s">
         <v>7</v>
       </c>
@@ -3089,11 +3164,11 @@
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="48"/>
-      <c r="B30" s="49" t="s">
+      <c r="A30" s="41"/>
+      <c r="B30" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="49" t="s">
+      <c r="C30" s="42" t="s">
         <v>118</v>
       </c>
       <c r="D30" s="10" t="s">
@@ -3104,9 +3179,9 @@
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="48"/>
-      <c r="B31" s="49"/>
-      <c r="C31" s="49"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
       <c r="D31" s="10" t="s">
         <v>7</v>
       </c>
@@ -3115,11 +3190,11 @@
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="48"/>
-      <c r="B32" s="49" t="s">
+      <c r="A32" s="41"/>
+      <c r="B32" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="49" t="s">
+      <c r="C32" s="42" t="s">
         <v>119</v>
       </c>
       <c r="D32" s="10" t="s">
@@ -3130,9 +3205,9 @@
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="48"/>
-      <c r="B33" s="49"/>
-      <c r="C33" s="49"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="42"/>
       <c r="D33" s="10" t="s">
         <v>7</v>
       </c>
@@ -3141,13 +3216,13 @@
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="43" t="s">
+      <c r="A34" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B34" s="43" t="s">
+      <c r="B34" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="43" t="s">
+      <c r="C34" s="44" t="s">
         <v>106</v>
       </c>
       <c r="D34" s="8" t="s">
@@ -3158,9 +3233,9 @@
       </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="43"/>
-      <c r="B35" s="43"/>
-      <c r="C35" s="43"/>
+      <c r="A35" s="44"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="44"/>
       <c r="D35" s="8" t="s">
         <v>7</v>
       </c>
@@ -3169,48 +3244,48 @@
       </c>
     </row>
     <row r="36" spans="1:5" hidden="1">
-      <c r="A36" s="43"/>
+      <c r="A36" s="44"/>
       <c r="B36" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="47"/>
-      <c r="D36" s="47"/>
+      <c r="C36" s="46"/>
+      <c r="D36" s="46"/>
       <c r="E36" s="8" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="43" t="s">
+      <c r="A37" s="44" t="s">
         <v>56</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="47" t="s">
+      <c r="C37" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="47"/>
-      <c r="E37" s="47"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
     </row>
     <row r="38" spans="1:5" hidden="1">
-      <c r="A38" s="43"/>
+      <c r="A38" s="44"/>
       <c r="B38" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C38" s="47"/>
-      <c r="D38" s="47"/>
+      <c r="C38" s="46"/>
+      <c r="D38" s="46"/>
       <c r="E38" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="43" t="s">
+      <c r="A39" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="43" t="s">
+      <c r="B39" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="43" t="s">
+      <c r="C39" s="44" t="s">
         <v>107</v>
       </c>
       <c r="D39" s="8" t="s">
@@ -3221,9 +3296,9 @@
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="43"/>
-      <c r="B40" s="43"/>
-      <c r="C40" s="43"/>
+      <c r="A40" s="44"/>
+      <c r="B40" s="44"/>
+      <c r="C40" s="44"/>
       <c r="D40" s="8" t="s">
         <v>7</v>
       </c>
@@ -3232,13 +3307,13 @@
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="43" t="s">
+      <c r="A41" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="B41" s="43" t="s">
+      <c r="B41" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="C41" s="43" t="s">
+      <c r="C41" s="44" t="s">
         <v>120</v>
       </c>
       <c r="D41" s="8" t="s">
@@ -3249,9 +3324,9 @@
       </c>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="43"/>
-      <c r="B42" s="43"/>
-      <c r="C42" s="43"/>
+      <c r="A42" s="44"/>
+      <c r="B42" s="44"/>
+      <c r="C42" s="44"/>
       <c r="D42" s="8" t="s">
         <v>7</v>
       </c>
@@ -3260,24 +3335,24 @@
       </c>
     </row>
     <row r="43" spans="1:5" hidden="1">
-      <c r="A43" s="43"/>
+      <c r="A43" s="44"/>
       <c r="B43" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C43" s="47"/>
-      <c r="D43" s="47"/>
+      <c r="C43" s="46"/>
+      <c r="D43" s="46"/>
       <c r="E43" s="8" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="48" t="s">
+      <c r="A44" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="B44" s="49" t="s">
+      <c r="B44" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="49" t="s">
+      <c r="C44" s="42" t="s">
         <v>108</v>
       </c>
       <c r="D44" s="10" t="s">
@@ -3288,9 +3363,9 @@
       </c>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="48"/>
-      <c r="B45" s="49"/>
-      <c r="C45" s="49"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="42"/>
+      <c r="C45" s="42"/>
       <c r="D45" s="10" t="s">
         <v>7</v>
       </c>
@@ -3299,53 +3374,53 @@
       </c>
     </row>
     <row r="46" spans="1:5" hidden="1">
-      <c r="A46" s="48"/>
+      <c r="A46" s="41"/>
       <c r="B46" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C46" s="46"/>
-      <c r="D46" s="46"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="43"/>
       <c r="E46" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:5" hidden="1">
-      <c r="A47" s="48"/>
+      <c r="A47" s="41"/>
       <c r="B47" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C47" s="46"/>
-      <c r="D47" s="46"/>
+      <c r="C47" s="43"/>
+      <c r="D47" s="43"/>
       <c r="E47" s="10" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15" customHeight="1">
-      <c r="A48" s="43" t="s">
+      <c r="A48" s="44" t="s">
         <v>45</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C48" s="44" t="s">
+      <c r="C48" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="D48" s="44"/>
-      <c r="E48" s="44"/>
+      <c r="D48" s="45"/>
+      <c r="E48" s="45"/>
     </row>
     <row r="49" spans="1:5" hidden="1">
-      <c r="A49" s="43"/>
+      <c r="A49" s="44"/>
       <c r="B49" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="44"/>
-      <c r="D49" s="44"/>
+      <c r="C49" s="45"/>
+      <c r="D49" s="45"/>
       <c r="E49" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="30">
-      <c r="A50" s="48" t="s">
+      <c r="A50" s="41" t="s">
         <v>87</v>
       </c>
       <c r="B50" s="10" t="s">
@@ -3362,11 +3437,11 @@
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="48"/>
-      <c r="B51" s="49" t="s">
+      <c r="A51" s="41"/>
+      <c r="B51" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="C51" s="50" t="s">
+      <c r="C51" s="47" t="s">
         <v>110</v>
       </c>
       <c r="D51" s="12" t="s">
@@ -3377,9 +3452,9 @@
       </c>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="48"/>
-      <c r="B52" s="49"/>
-      <c r="C52" s="50"/>
+      <c r="A52" s="41"/>
+      <c r="B52" s="42"/>
+      <c r="C52" s="47"/>
       <c r="D52" s="12" t="s">
         <v>7</v>
       </c>
@@ -3388,7 +3463,7 @@
       </c>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="48" t="s">
+      <c r="A53" s="41" t="s">
         <v>8</v>
       </c>
       <c r="B53" s="10" t="s">
@@ -3398,40 +3473,40 @@
         <v>111</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E53" s="10" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="54" spans="1:5" hidden="1">
-      <c r="A54" s="48"/>
+      <c r="A54" s="41"/>
       <c r="B54" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C54" s="46"/>
-      <c r="D54" s="46"/>
+      <c r="C54" s="43"/>
+      <c r="D54" s="43"/>
       <c r="E54" s="10" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:5" hidden="1">
-      <c r="A55" s="48"/>
+      <c r="A55" s="41"/>
       <c r="B55" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="46"/>
-      <c r="D55" s="46"/>
+      <c r="C55" s="43"/>
+      <c r="D55" s="43"/>
       <c r="E55" s="10" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="48"/>
-      <c r="B56" s="49" t="s">
+      <c r="A56" s="41"/>
+      <c r="B56" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="C56" s="49" t="s">
+      <c r="C56" s="42" t="s">
         <v>112</v>
       </c>
       <c r="D56" s="10" t="s">
@@ -3442,9 +3517,9 @@
       </c>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="48"/>
-      <c r="B57" s="49"/>
-      <c r="C57" s="49"/>
+      <c r="A57" s="41"/>
+      <c r="B57" s="42"/>
+      <c r="C57" s="42"/>
       <c r="D57" s="10" t="s">
         <v>7</v>
       </c>
@@ -3453,35 +3528,35 @@
       </c>
     </row>
     <row r="58" spans="1:5" hidden="1">
-      <c r="A58" s="48"/>
+      <c r="A58" s="41"/>
       <c r="B58" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C58" s="46"/>
-      <c r="D58" s="46"/>
+      <c r="C58" s="43"/>
+      <c r="D58" s="43"/>
       <c r="E58" s="10" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="59" spans="1:5" hidden="1">
-      <c r="A59" s="48"/>
+      <c r="A59" s="41"/>
       <c r="B59" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C59" s="46"/>
-      <c r="D59" s="46"/>
+      <c r="C59" s="43"/>
+      <c r="D59" s="43"/>
       <c r="E59" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="43" t="s">
+      <c r="A60" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="B60" s="43" t="s">
+      <c r="B60" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="C60" s="43" t="s">
+      <c r="C60" s="44" t="s">
         <v>113</v>
       </c>
       <c r="D60" s="8" t="s">
@@ -3492,9 +3567,9 @@
       </c>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="43"/>
-      <c r="B61" s="43"/>
-      <c r="C61" s="43"/>
+      <c r="A61" s="44"/>
+      <c r="B61" s="44"/>
+      <c r="C61" s="44"/>
       <c r="D61" s="8" t="s">
         <v>7</v>
       </c>
@@ -3503,72 +3578,72 @@
       </c>
     </row>
     <row r="62" spans="1:5" hidden="1">
-      <c r="A62" s="43"/>
+      <c r="A62" s="44"/>
       <c r="B62" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C62" s="47"/>
-      <c r="D62" s="47"/>
+      <c r="C62" s="46"/>
+      <c r="D62" s="46"/>
       <c r="E62" s="8" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="43" t="s">
+      <c r="A63" s="44" t="s">
         <v>56</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C63" s="47" t="s">
+      <c r="C63" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="D63" s="47"/>
-      <c r="E63" s="47"/>
+      <c r="D63" s="46"/>
+      <c r="E63" s="46"/>
     </row>
     <row r="64" spans="1:5" hidden="1">
-      <c r="A64" s="43"/>
+      <c r="A64" s="44"/>
       <c r="B64" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C64" s="47"/>
-      <c r="D64" s="47"/>
+      <c r="C64" s="46"/>
+      <c r="D64" s="46"/>
       <c r="E64" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="43" t="s">
+      <c r="A65" s="44" t="s">
         <v>65</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C65" s="47" t="s">
+      <c r="C65" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="D65" s="47"/>
-      <c r="E65" s="47"/>
+      <c r="D65" s="46"/>
+      <c r="E65" s="46"/>
     </row>
     <row r="66" spans="1:5" hidden="1">
-      <c r="A66" s="43"/>
+      <c r="A66" s="44"/>
       <c r="B66" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C66" s="47"/>
-      <c r="D66" s="47"/>
+      <c r="C66" s="46"/>
+      <c r="D66" s="46"/>
       <c r="E66" s="8" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="48" t="s">
+      <c r="A67" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="B67" s="49" t="s">
+      <c r="B67" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="C67" s="49" t="s">
+      <c r="C67" s="42" t="s">
         <v>114</v>
       </c>
       <c r="D67" s="10" t="s">
@@ -3579,9 +3654,9 @@
       </c>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="48"/>
-      <c r="B68" s="49"/>
-      <c r="C68" s="49"/>
+      <c r="A68" s="41"/>
+      <c r="B68" s="42"/>
+      <c r="C68" s="42"/>
       <c r="D68" s="10" t="s">
         <v>7</v>
       </c>
@@ -3590,53 +3665,53 @@
       </c>
     </row>
     <row r="69" spans="1:5" hidden="1">
-      <c r="A69" s="48"/>
+      <c r="A69" s="41"/>
       <c r="B69" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C69" s="46"/>
-      <c r="D69" s="46"/>
+      <c r="C69" s="43"/>
+      <c r="D69" s="43"/>
       <c r="E69" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="70" spans="1:5" hidden="1">
-      <c r="A70" s="48"/>
+      <c r="A70" s="41"/>
       <c r="B70" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C70" s="46"/>
-      <c r="D70" s="46"/>
+      <c r="C70" s="43"/>
+      <c r="D70" s="43"/>
       <c r="E70" s="10" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15" customHeight="1">
-      <c r="A71" s="43" t="s">
+      <c r="A71" s="44" t="s">
         <v>45</v>
       </c>
       <c r="B71" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C71" s="44" t="s">
+      <c r="C71" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="D71" s="44"/>
-      <c r="E71" s="44"/>
+      <c r="D71" s="45"/>
+      <c r="E71" s="45"/>
     </row>
     <row r="72" spans="1:5" hidden="1">
-      <c r="A72" s="43"/>
+      <c r="A72" s="44"/>
       <c r="B72" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C72" s="44"/>
-      <c r="D72" s="44"/>
+      <c r="C72" s="45"/>
+      <c r="D72" s="45"/>
       <c r="E72" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="45" t="s">
+      <c r="A73" s="48" t="s">
         <v>71</v>
       </c>
       <c r="B73" s="12" t="s">
@@ -3653,51 +3728,78 @@
       </c>
     </row>
     <row r="74" spans="1:5" hidden="1">
-      <c r="A74" s="45"/>
+      <c r="A74" s="48"/>
       <c r="B74" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C74" s="46"/>
-      <c r="D74" s="46"/>
+      <c r="C74" s="43"/>
+      <c r="D74" s="43"/>
       <c r="E74" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="75" spans="1:5" hidden="1">
-      <c r="A75" s="45"/>
+      <c r="A75" s="48"/>
       <c r="B75" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C75" s="46"/>
-      <c r="D75" s="46"/>
+      <c r="C75" s="43"/>
+      <c r="D75" s="43"/>
       <c r="E75" s="10" t="s">
         <v>74</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="87">
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="A73:A75"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="A67:A70"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="C30:C31"/>
     <mergeCell ref="B32:B33"/>
@@ -3714,55 +3816,28 @@
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="A67:A70"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="A73:A75"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <conditionalFormatting sqref="A76:E100">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="0">
@@ -3781,282 +3856,292 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="55.83203125" customWidth="1"/>
     <col min="2" max="2" width="20.83203125" style="14" customWidth="1"/>
-    <col min="3" max="4" width="55.83203125" style="24" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="31"/>
+    <col min="3" max="3" width="55.83203125" style="59" customWidth="1"/>
+    <col min="4" max="4" width="55.83203125" style="60" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="61" t="s">
         <v>145</v>
       </c>
-      <c r="B1" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="C1" s="22" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="30">
+      <c r="A2" s="53" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D2" s="57" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" s="50"/>
+      <c r="C3" s="49" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="30">
-      <c r="A2" s="27" t="s">
+      <c r="D3" s="56" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="50"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="57" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30">
+      <c r="A5" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="50"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="56" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="405" customHeight="1">
+      <c r="A6" s="54" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" s="50"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="58" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7" s="50"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="55" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="54" t="s">
+        <v>174</v>
+      </c>
+      <c r="B8" s="50"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="55"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" s="50"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="56"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" s="50"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="56"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" s="50"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="56" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" s="50"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="56" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30">
+      <c r="A13" s="53" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="D13" s="57" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30">
+      <c r="A14" s="53" t="s">
+        <v>127</v>
+      </c>
+      <c r="B14" s="26"/>
+      <c r="C14" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="B2" s="51" t="s">
-        <v>121</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>157</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="27" t="s">
-        <v>161</v>
-      </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="53" t="s">
-        <v>156</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="30" t="s">
+      <c r="D14" s="28" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15" s="50" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="51" t="s">
+        <v>144</v>
+      </c>
+      <c r="D15" s="56"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16" s="50"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="56"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="B17" s="50"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="56"/>
+    </row>
+    <row r="18" spans="1:4" ht="16" customHeight="1">
+      <c r="A18" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="B18" s="50"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="56"/>
+    </row>
+    <row r="19" spans="1:4" ht="30" customHeight="1">
+      <c r="A19" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="B19" s="50"/>
+      <c r="C19" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="D19" s="56"/>
+    </row>
+    <row r="20" spans="1:4" ht="75">
+      <c r="A20" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="D20" s="56"/>
+    </row>
+    <row r="21" spans="1:4" ht="240" customHeight="1">
+      <c r="A21" s="54" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="30">
-      <c r="A5" s="27" t="s">
-        <v>123</v>
-      </c>
-      <c r="B5" s="51"/>
-      <c r="C5" s="53"/>
-      <c r="D5" s="30" t="s">
+      <c r="B21" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="52" t="s">
+        <v>171</v>
+      </c>
+      <c r="D21" s="58" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="240" customHeight="1">
+      <c r="A22" s="54" t="s">
+        <v>164</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="52" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="375" customHeight="1">
-      <c r="A6" s="27" t="s">
-        <v>124</v>
-      </c>
-      <c r="B6" s="51"/>
-      <c r="C6" s="53"/>
-      <c r="D6" s="30" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="B7" s="51"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="30" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="60">
-      <c r="A8" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="B8" s="51"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="30" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="B9" s="51"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="30"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="B10" s="51"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="30" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="27" t="s">
-        <v>129</v>
-      </c>
-      <c r="B11" s="51"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="30" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30">
-      <c r="A12" s="27" t="s">
-        <v>162</v>
-      </c>
-      <c r="B12" s="54" t="s">
-        <v>131</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="D12" s="30" t="s">
+      <c r="D22" s="58" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30">
-      <c r="A13" s="27" t="s">
-        <v>130</v>
-      </c>
-      <c r="B13" s="54"/>
-      <c r="C13" s="29" t="s">
-        <v>153</v>
-      </c>
-      <c r="D13" s="33" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="27" t="s">
-        <v>132</v>
-      </c>
-      <c r="B14" s="51" t="s">
-        <v>133</v>
-      </c>
-      <c r="C14" s="52" t="s">
-        <v>149</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="B15" s="51"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="30" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="B16" s="51"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="30" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="16" customHeight="1">
-      <c r="A17" s="27" t="s">
+    <row r="23" spans="1:4">
+      <c r="A23" s="23" t="s">
         <v>136</v>
       </c>
-      <c r="B17" s="51"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="30" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="30" customHeight="1">
-      <c r="A18" s="27" t="s">
-        <v>140</v>
-      </c>
-      <c r="B18" s="51"/>
-      <c r="C18" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="D18" s="30" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="75">
-      <c r="A19" s="27" t="s">
+      <c r="B23" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="C23" s="31"/>
+      <c r="D23" s="56"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="C19" s="29" t="s">
-        <v>154</v>
-      </c>
-      <c r="D19" s="30" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="300">
-      <c r="A20" s="27" t="s">
+      <c r="B24" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="B20" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="C20" s="29" t="s">
-        <v>155</v>
-      </c>
-      <c r="D20" s="30" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="B21" s="27" t="s">
-        <v>142</v>
-      </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="30"/>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="B22" s="27" t="s">
-        <v>144</v>
-      </c>
-      <c r="C22" s="29"/>
-      <c r="D22" s="30"/>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="20"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="23"/>
-    </row>
-    <row r="39" ht="376" customHeight="1"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="56"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="20"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="62"/>
+    </row>
+    <row r="41" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B2:B11"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="C3:C11"/>
-    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C3:C12"/>
+    <mergeCell ref="B2:B12"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="D7:D8"/>
   </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
update linksPage and JobSeeker
add CRUD for CV
</commit_message>
<xml_diff>
--- a/linksPage.xlsx
+++ b/linksPage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15900" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15780" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="linkTable" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="181">
   <si>
     <t>request</t>
   </si>
@@ -410,27 +410,12 @@
     <t>fullAccountDto</t>
   </si>
   <si>
-    <t>POST /jobSeeker/activateResume</t>
-  </si>
-  <si>
-    <t>jobSeekerResumeDto</t>
-  </si>
-  <si>
-    <t>POST /jobSeeker/deactivateResume</t>
-  </si>
-  <si>
-    <t>POST /jobSeeker/removeResume</t>
-  </si>
-  <si>
     <t>POST /jobSeeker/editVisibility</t>
   </si>
   <si>
     <t>fieldsVisibilityDto</t>
   </si>
   <si>
-    <t>POST /jobSeeker/editResume</t>
-  </si>
-  <si>
     <t>POST /company/editProfile</t>
   </si>
   <si>
@@ -464,9 +449,6 @@
     <t>structure request</t>
   </si>
   <si>
-    <t>{"login":"my@email.com","yearsInWork":1,"skillsType":["java"],"companyName":["myCompany1"],"cvType":"backEnd"}</t>
-  </si>
-  <si>
     <t>{"login":"my@email.com","password":"1234567","typeQuestion":"question1","question":"answerToQuestion","phone":1234567}</t>
   </si>
   <si>
@@ -489,9 +471,6 @@
   </si>
   <si>
     <t>"notActivated" / "wrongCredentials" / "noSendEmail" / "false"</t>
-  </si>
-  <si>
-    <t>"ok" / "false"</t>
   </si>
   <si>
     <t>"ok" / "false" / "wrongRequest"</t>
@@ -519,12 +498,6 @@
     </r>
   </si>
   <si>
-    <t>POST /jobSeeker/getResumes</t>
-  </si>
-  <si>
-    <t>POST /jobSeeker/verifyResume/inProcess</t>
-  </si>
-  <si>
     <t>POST /jobSeeker/createProfile</t>
   </si>
   <si>
@@ -556,13 +529,58 @@
   </si>
   <si>
     <t>POST /jobSeeker/restoreProfile</t>
+  </si>
+  <si>
+    <t>POST /jobSeeker/createCv</t>
+  </si>
+  <si>
+    <t>{"login":"my@email.com","cvType":"backEnd","yearsInWork":1,"skillsType":["java"],"companyName":["myCompany1"],"minSalary":1}</t>
+  </si>
+  <si>
+    <t>POST /jobSeeker/verifyCv/inProcess</t>
+  </si>
+  <si>
+    <t>POST /jobSeeker/updateCv</t>
+  </si>
+  <si>
+    <t>POST /jobSeeker/readCv</t>
+  </si>
+  <si>
+    <t>POST /jobSeeker/readAllCv</t>
+  </si>
+  <si>
+    <t>"ok" / "wrongRequest" / "noFounf" / "exist"</t>
+  </si>
+  <si>
+    <t>"noFound" / "ok"</t>
+  </si>
+  <si>
+    <t>POST /jobSeeker/deleteCv</t>
+  </si>
+  <si>
+    <t>POST /jobSeeker/enableCv</t>
+  </si>
+  <si>
+    <t>POST /jobSeeker/enableAllCv</t>
+  </si>
+  <si>
+    <t>POST /jobSeeker/disableCv</t>
+  </si>
+  <si>
+    <t>jobSeekerCvDto</t>
+  </si>
+  <si>
+    <t>"noFound" / "false" {"login":"my@Email.com","yearsInWork":1,"skillsType":["java"],"companyName":["myCompany1"],"verification":{"date":"","verificationStatus":"no"},"cvType":"backEnd","dateOfEnable":"2017-12-18","enable":true,"minSalary":1}</t>
+  </si>
+  <si>
+    <t>"noFound" / "false" [{"login":"my@Email.com","yearsInWork":1,"skillsType":["java"],"companyName":["myCompany1"],"verification":{"date":"","verificationStatus":"no"},"cvType":"backEnd","dateOfEnable":"2017-12-18","enable":true,"minSalary":1}]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -624,8 +642,16 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -652,12 +678,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -665,8 +697,110 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="249">
+  <cellStyleXfs count="289">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -916,8 +1050,48 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -973,16 +1147,9 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -990,119 +1157,230 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="249">
+  <cellStyles count="289">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="5" builtinId="8" hidden="1"/>
@@ -1227,6 +1505,26 @@
     <cellStyle name="Гиперссылка" xfId="243" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="245" builtinId="8" hidden="1"/>
     <cellStyle name="Гиперссылка" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Гиперссылка" xfId="287" builtinId="8" hidden="1"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="4" builtinId="9" hidden="1"/>
@@ -1352,6 +1650,26 @@
     <cellStyle name="Просмотренная гиперссылка" xfId="244" builtinId="9" hidden="1"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="246" builtinId="9" hidden="1"/>
     <cellStyle name="Просмотренная гиперссылка" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Просмотренная гиперссылка" xfId="288" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1731,14 +2049,14 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="36" t="s">
-        <v>142</v>
+      <c r="C2" s="67" t="s">
+        <v>137</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>3</v>
@@ -1748,9 +2066,9 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
-      <c r="A3" s="34"/>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
+      <c r="A3" s="65"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
       <c r="D3" s="15" t="s">
         <v>2</v>
       </c>
@@ -1759,9 +2077,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1">
-      <c r="A4" s="34"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
+      <c r="A4" s="65"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
       <c r="D4" s="15" t="s">
         <v>4</v>
       </c>
@@ -1770,9 +2088,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1">
-      <c r="A5" s="34"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
       <c r="D5" s="15" t="s">
         <v>5</v>
       </c>
@@ -1781,59 +2099,59 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1">
-      <c r="A6" s="34"/>
+      <c r="A6" s="65"/>
       <c r="B6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
       <c r="E6" s="15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="66" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="35" t="s">
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="66" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1">
-      <c r="A8" s="35"/>
+      <c r="A8" s="66"/>
       <c r="B8" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="35"/>
+      <c r="E8" s="66"/>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="66" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
       <c r="E9" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1">
-      <c r="A10" s="35"/>
+      <c r="A10" s="66"/>
       <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
       <c r="E10" s="1" t="s">
         <v>28</v>
       </c>
@@ -1854,13 +2172,13 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="67" t="s">
         <v>104</v>
       </c>
       <c r="D12" s="15" t="s">
@@ -1871,9 +2189,9 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1">
-      <c r="A13" s="34"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
+      <c r="A13" s="65"/>
+      <c r="B13" s="67"/>
+      <c r="C13" s="67"/>
       <c r="D13" s="15" t="s">
         <v>5</v>
       </c>
@@ -1882,9 +2200,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1">
-      <c r="A14" s="34"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
+      <c r="A14" s="65"/>
+      <c r="B14" s="67"/>
+      <c r="C14" s="67"/>
       <c r="D14" s="15" t="s">
         <v>7</v>
       </c>
@@ -1899,62 +2217,62 @@
       <c r="B15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
       <c r="E15" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="66" t="s">
         <v>39</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
       <c r="E16" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1">
-      <c r="A17" s="35"/>
+      <c r="A17" s="66"/>
       <c r="B17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="69"/>
       <c r="E17" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="66" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="70" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="70"/>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1">
-      <c r="A19" s="35"/>
+      <c r="A19" s="66"/>
       <c r="B19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
       <c r="E19" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="65" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="15" t="s">
@@ -1971,88 +2289,88 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1">
-      <c r="A21" s="34"/>
+      <c r="A21" s="65"/>
       <c r="B21" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="67"/>
       <c r="E21" s="15" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1">
-      <c r="A22" s="34"/>
+      <c r="A22" s="65"/>
       <c r="B22" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="67"/>
       <c r="E22" s="15" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1">
-      <c r="A23" s="34"/>
+      <c r="A23" s="65"/>
       <c r="B23" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67"/>
       <c r="E23" s="15" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1">
-      <c r="A24" s="34"/>
+      <c r="A24" s="65"/>
       <c r="B24" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="67"/>
       <c r="E24" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1">
-      <c r="A25" s="34"/>
+      <c r="A25" s="65"/>
       <c r="B25" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="63"/>
       <c r="E25" s="15" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1">
-      <c r="A26" s="34"/>
+      <c r="A26" s="65"/>
       <c r="B26" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="63"/>
       <c r="E26" s="15" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1">
-      <c r="A27" s="34"/>
+      <c r="A27" s="65"/>
       <c r="B27" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
+      <c r="C27" s="63"/>
+      <c r="D27" s="63"/>
       <c r="E27" s="15" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" customHeight="1">
-      <c r="A28" s="34"/>
-      <c r="B28" s="36" t="s">
+      <c r="A28" s="65"/>
+      <c r="B28" s="67" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="36" t="s">
+      <c r="C28" s="67" t="s">
         <v>117</v>
       </c>
       <c r="D28" s="16" t="s">
@@ -2063,9 +2381,9 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" customHeight="1">
-      <c r="A29" s="34"/>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
+      <c r="A29" s="65"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="67"/>
       <c r="D29" s="15" t="s">
         <v>7</v>
       </c>
@@ -2074,11 +2392,11 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" customHeight="1">
-      <c r="A30" s="34"/>
-      <c r="B30" s="36" t="s">
+      <c r="A30" s="65"/>
+      <c r="B30" s="67" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="36" t="s">
+      <c r="C30" s="67" t="s">
         <v>118</v>
       </c>
       <c r="D30" s="15" t="s">
@@ -2089,9 +2407,9 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="15" customHeight="1">
-      <c r="A31" s="34"/>
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
+      <c r="A31" s="65"/>
+      <c r="B31" s="67"/>
+      <c r="C31" s="67"/>
       <c r="D31" s="15" t="s">
         <v>7</v>
       </c>
@@ -2100,11 +2418,11 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" customHeight="1">
-      <c r="A32" s="34"/>
-      <c r="B32" s="36" t="s">
+      <c r="A32" s="65"/>
+      <c r="B32" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="36" t="s">
+      <c r="C32" s="67" t="s">
         <v>119</v>
       </c>
       <c r="D32" s="15" t="s">
@@ -2115,9 +2433,9 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" customHeight="1">
-      <c r="A33" s="34"/>
-      <c r="B33" s="36"/>
-      <c r="C33" s="36"/>
+      <c r="A33" s="65"/>
+      <c r="B33" s="67"/>
+      <c r="C33" s="67"/>
       <c r="D33" s="15" t="s">
         <v>7</v>
       </c>
@@ -2126,13 +2444,13 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" customHeight="1">
-      <c r="A34" s="35" t="s">
+      <c r="A34" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="35" t="s">
+      <c r="C34" s="66" t="s">
         <v>106</v>
       </c>
       <c r="D34" s="1" t="s">
@@ -2143,9 +2461,9 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" customHeight="1">
-      <c r="A35" s="35"/>
-      <c r="B35" s="35"/>
-      <c r="C35" s="35"/>
+      <c r="A35" s="66"/>
+      <c r="B35" s="66"/>
+      <c r="C35" s="66"/>
       <c r="D35" s="1" t="s">
         <v>7</v>
       </c>
@@ -2154,48 +2472,48 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" customHeight="1">
-      <c r="A36" s="35"/>
+      <c r="A36" s="66"/>
       <c r="B36" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
+      <c r="C36" s="69"/>
+      <c r="D36" s="69"/>
       <c r="E36" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" customHeight="1">
-      <c r="A37" s="35" t="s">
+      <c r="A37" s="66" t="s">
         <v>56</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="38" t="s">
+      <c r="C37" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="38"/>
-      <c r="E37" s="38"/>
+      <c r="D37" s="69"/>
+      <c r="E37" s="69"/>
     </row>
     <row r="38" spans="1:5" ht="15" customHeight="1">
-      <c r="A38" s="35"/>
+      <c r="A38" s="66"/>
       <c r="B38" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C38" s="38"/>
-      <c r="D38" s="38"/>
+      <c r="C38" s="69"/>
+      <c r="D38" s="69"/>
       <c r="E38" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15" customHeight="1">
-      <c r="A39" s="35" t="s">
+      <c r="A39" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="35" t="s">
+      <c r="B39" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="35" t="s">
+      <c r="C39" s="66" t="s">
         <v>107</v>
       </c>
       <c r="D39" s="1" t="s">
@@ -2206,9 +2524,9 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="15" customHeight="1">
-      <c r="A40" s="35"/>
-      <c r="B40" s="35"/>
-      <c r="C40" s="35"/>
+      <c r="A40" s="66"/>
+      <c r="B40" s="66"/>
+      <c r="C40" s="66"/>
       <c r="D40" s="1" t="s">
         <v>7</v>
       </c>
@@ -2217,13 +2535,13 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="15" customHeight="1">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="66" t="s">
         <v>97</v>
       </c>
-      <c r="B41" s="35" t="s">
+      <c r="B41" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="C41" s="35" t="s">
+      <c r="C41" s="66" t="s">
         <v>120</v>
       </c>
       <c r="D41" s="1" t="s">
@@ -2234,9 +2552,9 @@
       </c>
     </row>
     <row r="42" spans="1:5" ht="15" customHeight="1">
-      <c r="A42" s="35"/>
-      <c r="B42" s="35"/>
-      <c r="C42" s="35"/>
+      <c r="A42" s="66"/>
+      <c r="B42" s="66"/>
+      <c r="C42" s="66"/>
       <c r="D42" s="1" t="s">
         <v>7</v>
       </c>
@@ -2245,24 +2563,24 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" customHeight="1">
-      <c r="A43" s="35"/>
+      <c r="A43" s="66"/>
       <c r="B43" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
+      <c r="C43" s="69"/>
+      <c r="D43" s="69"/>
       <c r="E43" s="1" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15" customHeight="1">
-      <c r="A44" s="34" t="s">
+      <c r="A44" s="65" t="s">
         <v>73</v>
       </c>
-      <c r="B44" s="36" t="s">
+      <c r="B44" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="36" t="s">
+      <c r="C44" s="67" t="s">
         <v>108</v>
       </c>
       <c r="D44" s="15" t="s">
@@ -2273,9 +2591,9 @@
       </c>
     </row>
     <row r="45" spans="1:5" ht="15" customHeight="1">
-      <c r="A45" s="34"/>
-      <c r="B45" s="36"/>
-      <c r="C45" s="36"/>
+      <c r="A45" s="65"/>
+      <c r="B45" s="67"/>
+      <c r="C45" s="67"/>
       <c r="D45" s="15" t="s">
         <v>7</v>
       </c>
@@ -2284,53 +2602,53 @@
       </c>
     </row>
     <row r="46" spans="1:5" ht="15" customHeight="1">
-      <c r="A46" s="34"/>
+      <c r="A46" s="65"/>
       <c r="B46" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C46" s="32"/>
-      <c r="D46" s="32"/>
+      <c r="C46" s="63"/>
+      <c r="D46" s="63"/>
       <c r="E46" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15" customHeight="1">
-      <c r="A47" s="34"/>
+      <c r="A47" s="65"/>
       <c r="B47" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C47" s="32"/>
-      <c r="D47" s="32"/>
+      <c r="C47" s="63"/>
+      <c r="D47" s="63"/>
       <c r="E47" s="15" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15" customHeight="1">
-      <c r="A48" s="35" t="s">
+      <c r="A48" s="66" t="s">
         <v>45</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C48" s="37" t="s">
+      <c r="C48" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="D48" s="37"/>
-      <c r="E48" s="37"/>
+      <c r="D48" s="68"/>
+      <c r="E48" s="68"/>
     </row>
     <row r="49" spans="1:5" ht="15" customHeight="1">
-      <c r="A49" s="35"/>
+      <c r="A49" s="66"/>
       <c r="B49" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="37"/>
-      <c r="D49" s="37"/>
+      <c r="C49" s="68"/>
+      <c r="D49" s="68"/>
       <c r="E49" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="30" customHeight="1">
-      <c r="A50" s="34" t="s">
+      <c r="A50" s="65" t="s">
         <v>87</v>
       </c>
       <c r="B50" s="15" t="s">
@@ -2347,11 +2665,11 @@
       </c>
     </row>
     <row r="51" spans="1:5" ht="15" customHeight="1">
-      <c r="A51" s="34"/>
-      <c r="B51" s="36" t="s">
+      <c r="A51" s="65"/>
+      <c r="B51" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="C51" s="40" t="s">
+      <c r="C51" s="71" t="s">
         <v>110</v>
       </c>
       <c r="D51" s="17" t="s">
@@ -2362,9 +2680,9 @@
       </c>
     </row>
     <row r="52" spans="1:5" ht="15" customHeight="1">
-      <c r="A52" s="34"/>
-      <c r="B52" s="36"/>
-      <c r="C52" s="40"/>
+      <c r="A52" s="65"/>
+      <c r="B52" s="67"/>
+      <c r="C52" s="71"/>
       <c r="D52" s="17" t="s">
         <v>7</v>
       </c>
@@ -2373,7 +2691,7 @@
       </c>
     </row>
     <row r="53" spans="1:5" ht="15" customHeight="1">
-      <c r="A53" s="34" t="s">
+      <c r="A53" s="65" t="s">
         <v>8</v>
       </c>
       <c r="B53" s="15" t="s">
@@ -2383,40 +2701,40 @@
         <v>111</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E53" s="15" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15" customHeight="1">
-      <c r="A54" s="34"/>
+      <c r="A54" s="65"/>
       <c r="B54" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C54" s="32"/>
-      <c r="D54" s="32"/>
+      <c r="C54" s="63"/>
+      <c r="D54" s="63"/>
       <c r="E54" s="15" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15" customHeight="1">
-      <c r="A55" s="34"/>
+      <c r="A55" s="65"/>
       <c r="B55" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="32"/>
-      <c r="D55" s="32"/>
+      <c r="C55" s="63"/>
+      <c r="D55" s="63"/>
       <c r="E55" s="15" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15" customHeight="1">
-      <c r="A56" s="34"/>
-      <c r="B56" s="36" t="s">
+      <c r="A56" s="65"/>
+      <c r="B56" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="C56" s="36" t="s">
+      <c r="C56" s="67" t="s">
         <v>112</v>
       </c>
       <c r="D56" s="15" t="s">
@@ -2427,9 +2745,9 @@
       </c>
     </row>
     <row r="57" spans="1:5" ht="15" customHeight="1">
-      <c r="A57" s="34"/>
-      <c r="B57" s="36"/>
-      <c r="C57" s="36"/>
+      <c r="A57" s="65"/>
+      <c r="B57" s="67"/>
+      <c r="C57" s="67"/>
       <c r="D57" s="15" t="s">
         <v>7</v>
       </c>
@@ -2438,35 +2756,35 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="15" customHeight="1">
-      <c r="A58" s="34"/>
+      <c r="A58" s="65"/>
       <c r="B58" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C58" s="32"/>
-      <c r="D58" s="32"/>
+      <c r="C58" s="63"/>
+      <c r="D58" s="63"/>
       <c r="E58" s="15" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15" customHeight="1">
-      <c r="A59" s="34"/>
+      <c r="A59" s="65"/>
       <c r="B59" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C59" s="32"/>
-      <c r="D59" s="32"/>
+      <c r="C59" s="63"/>
+      <c r="D59" s="63"/>
       <c r="E59" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15" customHeight="1">
-      <c r="A60" s="35" t="s">
+      <c r="A60" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="B60" s="35" t="s">
+      <c r="B60" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="C60" s="35" t="s">
+      <c r="C60" s="66" t="s">
         <v>113</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -2477,9 +2795,9 @@
       </c>
     </row>
     <row r="61" spans="1:5" ht="15" customHeight="1">
-      <c r="A61" s="35"/>
-      <c r="B61" s="35"/>
-      <c r="C61" s="35"/>
+      <c r="A61" s="66"/>
+      <c r="B61" s="66"/>
+      <c r="C61" s="66"/>
       <c r="D61" s="1" t="s">
         <v>7</v>
       </c>
@@ -2488,72 +2806,72 @@
       </c>
     </row>
     <row r="62" spans="1:5" ht="15" customHeight="1">
-      <c r="A62" s="35"/>
+      <c r="A62" s="66"/>
       <c r="B62" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C62" s="38"/>
-      <c r="D62" s="38"/>
+      <c r="C62" s="69"/>
+      <c r="D62" s="69"/>
       <c r="E62" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="15" customHeight="1">
-      <c r="A63" s="35" t="s">
+      <c r="A63" s="66" t="s">
         <v>56</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C63" s="38" t="s">
+      <c r="C63" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="D63" s="38"/>
-      <c r="E63" s="38"/>
+      <c r="D63" s="69"/>
+      <c r="E63" s="69"/>
     </row>
     <row r="64" spans="1:5" ht="15" customHeight="1">
-      <c r="A64" s="35"/>
+      <c r="A64" s="66"/>
       <c r="B64" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C64" s="38"/>
-      <c r="D64" s="38"/>
+      <c r="C64" s="69"/>
+      <c r="D64" s="69"/>
       <c r="E64" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="15" customHeight="1">
-      <c r="A65" s="35" t="s">
+      <c r="A65" s="66" t="s">
         <v>65</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C65" s="38" t="s">
+      <c r="C65" s="69" t="s">
         <v>66</v>
       </c>
-      <c r="D65" s="38"/>
-      <c r="E65" s="38"/>
+      <c r="D65" s="69"/>
+      <c r="E65" s="69"/>
     </row>
     <row r="66" spans="1:5" ht="15" customHeight="1">
-      <c r="A66" s="35"/>
+      <c r="A66" s="66"/>
       <c r="B66" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C66" s="38"/>
-      <c r="D66" s="38"/>
+      <c r="C66" s="69"/>
+      <c r="D66" s="69"/>
       <c r="E66" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="15" customHeight="1">
-      <c r="A67" s="34" t="s">
+      <c r="A67" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="B67" s="36" t="s">
+      <c r="B67" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="C67" s="36" t="s">
+      <c r="C67" s="67" t="s">
         <v>114</v>
       </c>
       <c r="D67" s="15" t="s">
@@ -2564,9 +2882,9 @@
       </c>
     </row>
     <row r="68" spans="1:5" ht="15" customHeight="1">
-      <c r="A68" s="34"/>
-      <c r="B68" s="36"/>
-      <c r="C68" s="36"/>
+      <c r="A68" s="65"/>
+      <c r="B68" s="67"/>
+      <c r="C68" s="67"/>
       <c r="D68" s="15" t="s">
         <v>7</v>
       </c>
@@ -2575,53 +2893,53 @@
       </c>
     </row>
     <row r="69" spans="1:5" ht="15" customHeight="1">
-      <c r="A69" s="34"/>
+      <c r="A69" s="65"/>
       <c r="B69" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C69" s="32"/>
-      <c r="D69" s="32"/>
+      <c r="C69" s="63"/>
+      <c r="D69" s="63"/>
       <c r="E69" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="15" customHeight="1">
-      <c r="A70" s="34"/>
+      <c r="A70" s="65"/>
       <c r="B70" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C70" s="32"/>
-      <c r="D70" s="32"/>
+      <c r="C70" s="63"/>
+      <c r="D70" s="63"/>
       <c r="E70" s="15" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15" customHeight="1">
-      <c r="A71" s="35" t="s">
+      <c r="A71" s="66" t="s">
         <v>45</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C71" s="37" t="s">
+      <c r="C71" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="D71" s="37"/>
-      <c r="E71" s="37"/>
+      <c r="D71" s="68"/>
+      <c r="E71" s="68"/>
     </row>
     <row r="72" spans="1:5" ht="15" customHeight="1">
-      <c r="A72" s="35"/>
+      <c r="A72" s="66"/>
       <c r="B72" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C72" s="37"/>
-      <c r="D72" s="37"/>
+      <c r="C72" s="68"/>
+      <c r="D72" s="68"/>
       <c r="E72" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="15" customHeight="1">
-      <c r="A73" s="33" t="s">
+      <c r="A73" s="64" t="s">
         <v>71</v>
       </c>
       <c r="B73" s="17" t="s">
@@ -2638,23 +2956,23 @@
       </c>
     </row>
     <row r="74" spans="1:5" ht="15" customHeight="1">
-      <c r="A74" s="33"/>
+      <c r="A74" s="64"/>
       <c r="B74" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C74" s="32"/>
-      <c r="D74" s="32"/>
+      <c r="C74" s="63"/>
+      <c r="D74" s="63"/>
       <c r="E74" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="15" customHeight="1">
-      <c r="A75" s="33"/>
+      <c r="A75" s="64"/>
       <c r="B75" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C75" s="32"/>
-      <c r="D75" s="32"/>
+      <c r="C75" s="63"/>
+      <c r="D75" s="63"/>
       <c r="E75" s="15" t="s">
         <v>74</v>
       </c>
@@ -2820,13 +3138,13 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="73" t="s">
         <v>101</v>
       </c>
       <c r="D2" s="10" t="s">
@@ -2837,9 +3155,9 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="41"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
+      <c r="A3" s="72"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
       <c r="D3" s="10" t="s">
         <v>2</v>
       </c>
@@ -2848,9 +3166,9 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="41"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
+      <c r="A4" s="72"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
       <c r="D4" s="10" t="s">
         <v>4</v>
       </c>
@@ -2859,9 +3177,9 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="41"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
+      <c r="A5" s="72"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
       <c r="D5" s="10" t="s">
         <v>5</v>
       </c>
@@ -2870,31 +3188,31 @@
       </c>
     </row>
     <row r="6" spans="1:5" hidden="1">
-      <c r="A6" s="41"/>
+      <c r="A6" s="72"/>
       <c r="B6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
       <c r="E6" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" hidden="1">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="75" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="44" t="s">
+      <c r="C7" s="76"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="75" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="44"/>
+      <c r="A8" s="75"/>
       <c r="B8" s="8" t="s">
         <v>24</v>
       </c>
@@ -2902,28 +3220,28 @@
         <v>102</v>
       </c>
       <c r="D8" s="8"/>
-      <c r="E8" s="44"/>
+      <c r="E8" s="75"/>
     </row>
     <row r="9" spans="1:5" hidden="1">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="75" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
+      <c r="C9" s="77"/>
+      <c r="D9" s="77"/>
       <c r="E9" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:5" hidden="1">
-      <c r="A10" s="44"/>
+      <c r="A10" s="75"/>
       <c r="B10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="77"/>
       <c r="E10" s="8" t="s">
         <v>28</v>
       </c>
@@ -2944,13 +3262,13 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="73" t="s">
         <v>104</v>
       </c>
       <c r="D12" s="10" t="s">
@@ -2961,9 +3279,9 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="41"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="42"/>
+      <c r="A13" s="72"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
       <c r="D13" s="10" t="s">
         <v>5</v>
       </c>
@@ -2972,9 +3290,9 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="41"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
+      <c r="A14" s="72"/>
+      <c r="B14" s="73"/>
+      <c r="C14" s="73"/>
       <c r="D14" s="10" t="s">
         <v>7</v>
       </c>
@@ -2989,62 +3307,62 @@
       <c r="B15" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
+      <c r="C15" s="77"/>
+      <c r="D15" s="77"/>
       <c r="E15" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:5" hidden="1">
-      <c r="A16" s="44" t="s">
+      <c r="A16" s="75" t="s">
         <v>39</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="77"/>
       <c r="E16" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:5" hidden="1">
-      <c r="A17" s="44"/>
+      <c r="A17" s="75"/>
       <c r="B17" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="77"/>
       <c r="E17" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="75" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="45" t="s">
+      <c r="C18" s="76" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="76"/>
     </row>
     <row r="19" spans="1:5" hidden="1">
-      <c r="A19" s="44"/>
+      <c r="A19" s="75"/>
       <c r="B19" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
+      <c r="C19" s="77"/>
+      <c r="D19" s="77"/>
       <c r="E19" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="72" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="10" t="s">
@@ -3061,88 +3379,88 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1">
-      <c r="A21" s="41"/>
+      <c r="A21" s="72"/>
       <c r="B21" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
+      <c r="C21" s="73"/>
+      <c r="D21" s="73"/>
       <c r="E21" s="10" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:5" hidden="1">
-      <c r="A22" s="41"/>
+      <c r="A22" s="72"/>
       <c r="B22" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="73"/>
       <c r="E22" s="10" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1">
-      <c r="A23" s="41"/>
+      <c r="A23" s="72"/>
       <c r="B23" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
+      <c r="C23" s="73"/>
+      <c r="D23" s="73"/>
       <c r="E23" s="10" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1">
-      <c r="A24" s="41"/>
+      <c r="A24" s="72"/>
       <c r="B24" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
+      <c r="C24" s="73"/>
+      <c r="D24" s="73"/>
       <c r="E24" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:5" hidden="1">
-      <c r="A25" s="41"/>
+      <c r="A25" s="72"/>
       <c r="B25" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
+      <c r="C25" s="74"/>
+      <c r="D25" s="74"/>
       <c r="E25" s="10" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:5" hidden="1">
-      <c r="A26" s="41"/>
+      <c r="A26" s="72"/>
       <c r="B26" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
+      <c r="C26" s="74"/>
+      <c r="D26" s="74"/>
       <c r="E26" s="10" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:5" hidden="1">
-      <c r="A27" s="41"/>
+      <c r="A27" s="72"/>
       <c r="B27" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
+      <c r="C27" s="74"/>
+      <c r="D27" s="74"/>
       <c r="E27" s="10" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="41"/>
-      <c r="B28" s="42" t="s">
+      <c r="A28" s="72"/>
+      <c r="B28" s="73" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="42" t="s">
+      <c r="C28" s="73" t="s">
         <v>117</v>
       </c>
       <c r="D28" s="11" t="s">
@@ -3153,9 +3471,9 @@
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="41"/>
-      <c r="B29" s="42"/>
-      <c r="C29" s="42"/>
+      <c r="A29" s="72"/>
+      <c r="B29" s="73"/>
+      <c r="C29" s="73"/>
       <c r="D29" s="10" t="s">
         <v>7</v>
       </c>
@@ -3164,11 +3482,11 @@
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="41"/>
-      <c r="B30" s="42" t="s">
+      <c r="A30" s="72"/>
+      <c r="B30" s="73" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="42" t="s">
+      <c r="C30" s="73" t="s">
         <v>118</v>
       </c>
       <c r="D30" s="10" t="s">
@@ -3179,9 +3497,9 @@
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="41"/>
-      <c r="B31" s="42"/>
-      <c r="C31" s="42"/>
+      <c r="A31" s="72"/>
+      <c r="B31" s="73"/>
+      <c r="C31" s="73"/>
       <c r="D31" s="10" t="s">
         <v>7</v>
       </c>
@@ -3190,11 +3508,11 @@
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="41"/>
-      <c r="B32" s="42" t="s">
+      <c r="A32" s="72"/>
+      <c r="B32" s="73" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="42" t="s">
+      <c r="C32" s="73" t="s">
         <v>119</v>
       </c>
       <c r="D32" s="10" t="s">
@@ -3205,9 +3523,9 @@
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="41"/>
-      <c r="B33" s="42"/>
-      <c r="C33" s="42"/>
+      <c r="A33" s="72"/>
+      <c r="B33" s="73"/>
+      <c r="C33" s="73"/>
       <c r="D33" s="10" t="s">
         <v>7</v>
       </c>
@@ -3216,13 +3534,13 @@
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="44" t="s">
+      <c r="A34" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="B34" s="44" t="s">
+      <c r="B34" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="44" t="s">
+      <c r="C34" s="75" t="s">
         <v>106</v>
       </c>
       <c r="D34" s="8" t="s">
@@ -3233,9 +3551,9 @@
       </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="44"/>
-      <c r="B35" s="44"/>
-      <c r="C35" s="44"/>
+      <c r="A35" s="75"/>
+      <c r="B35" s="75"/>
+      <c r="C35" s="75"/>
       <c r="D35" s="8" t="s">
         <v>7</v>
       </c>
@@ -3244,48 +3562,48 @@
       </c>
     </row>
     <row r="36" spans="1:5" hidden="1">
-      <c r="A36" s="44"/>
+      <c r="A36" s="75"/>
       <c r="B36" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="46"/>
-      <c r="D36" s="46"/>
+      <c r="C36" s="77"/>
+      <c r="D36" s="77"/>
       <c r="E36" s="8" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="44" t="s">
+      <c r="A37" s="75" t="s">
         <v>56</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="46" t="s">
+      <c r="C37" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="46"/>
-      <c r="E37" s="46"/>
+      <c r="D37" s="77"/>
+      <c r="E37" s="77"/>
     </row>
     <row r="38" spans="1:5" hidden="1">
-      <c r="A38" s="44"/>
+      <c r="A38" s="75"/>
       <c r="B38" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C38" s="46"/>
-      <c r="D38" s="46"/>
+      <c r="C38" s="77"/>
+      <c r="D38" s="77"/>
       <c r="E38" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="44" t="s">
+      <c r="A39" s="75" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="44" t="s">
+      <c r="B39" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="44" t="s">
+      <c r="C39" s="75" t="s">
         <v>107</v>
       </c>
       <c r="D39" s="8" t="s">
@@ -3296,9 +3614,9 @@
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="44"/>
-      <c r="B40" s="44"/>
-      <c r="C40" s="44"/>
+      <c r="A40" s="75"/>
+      <c r="B40" s="75"/>
+      <c r="C40" s="75"/>
       <c r="D40" s="8" t="s">
         <v>7</v>
       </c>
@@ -3307,13 +3625,13 @@
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="44" t="s">
+      <c r="A41" s="75" t="s">
         <v>97</v>
       </c>
-      <c r="B41" s="44" t="s">
+      <c r="B41" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="C41" s="44" t="s">
+      <c r="C41" s="75" t="s">
         <v>120</v>
       </c>
       <c r="D41" s="8" t="s">
@@ -3324,9 +3642,9 @@
       </c>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="44"/>
-      <c r="B42" s="44"/>
-      <c r="C42" s="44"/>
+      <c r="A42" s="75"/>
+      <c r="B42" s="75"/>
+      <c r="C42" s="75"/>
       <c r="D42" s="8" t="s">
         <v>7</v>
       </c>
@@ -3335,24 +3653,24 @@
       </c>
     </row>
     <row r="43" spans="1:5" hidden="1">
-      <c r="A43" s="44"/>
+      <c r="A43" s="75"/>
       <c r="B43" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C43" s="46"/>
-      <c r="D43" s="46"/>
+      <c r="C43" s="77"/>
+      <c r="D43" s="77"/>
       <c r="E43" s="8" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="41" t="s">
+      <c r="A44" s="72" t="s">
         <v>73</v>
       </c>
-      <c r="B44" s="42" t="s">
+      <c r="B44" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="42" t="s">
+      <c r="C44" s="73" t="s">
         <v>108</v>
       </c>
       <c r="D44" s="10" t="s">
@@ -3363,9 +3681,9 @@
       </c>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="41"/>
-      <c r="B45" s="42"/>
-      <c r="C45" s="42"/>
+      <c r="A45" s="72"/>
+      <c r="B45" s="73"/>
+      <c r="C45" s="73"/>
       <c r="D45" s="10" t="s">
         <v>7</v>
       </c>
@@ -3374,53 +3692,53 @@
       </c>
     </row>
     <row r="46" spans="1:5" hidden="1">
-      <c r="A46" s="41"/>
+      <c r="A46" s="72"/>
       <c r="B46" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C46" s="43"/>
-      <c r="D46" s="43"/>
+      <c r="C46" s="74"/>
+      <c r="D46" s="74"/>
       <c r="E46" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:5" hidden="1">
-      <c r="A47" s="41"/>
+      <c r="A47" s="72"/>
       <c r="B47" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C47" s="43"/>
-      <c r="D47" s="43"/>
+      <c r="C47" s="74"/>
+      <c r="D47" s="74"/>
       <c r="E47" s="10" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15" customHeight="1">
-      <c r="A48" s="44" t="s">
+      <c r="A48" s="75" t="s">
         <v>45</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C48" s="45" t="s">
+      <c r="C48" s="76" t="s">
         <v>57</v>
       </c>
-      <c r="D48" s="45"/>
-      <c r="E48" s="45"/>
+      <c r="D48" s="76"/>
+      <c r="E48" s="76"/>
     </row>
     <row r="49" spans="1:5" hidden="1">
-      <c r="A49" s="44"/>
+      <c r="A49" s="75"/>
       <c r="B49" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="45"/>
-      <c r="D49" s="45"/>
+      <c r="C49" s="76"/>
+      <c r="D49" s="76"/>
       <c r="E49" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="30">
-      <c r="A50" s="41" t="s">
+      <c r="A50" s="72" t="s">
         <v>87</v>
       </c>
       <c r="B50" s="10" t="s">
@@ -3437,11 +3755,11 @@
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="41"/>
-      <c r="B51" s="42" t="s">
+      <c r="A51" s="72"/>
+      <c r="B51" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="C51" s="47" t="s">
+      <c r="C51" s="78" t="s">
         <v>110</v>
       </c>
       <c r="D51" s="12" t="s">
@@ -3452,9 +3770,9 @@
       </c>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="41"/>
-      <c r="B52" s="42"/>
-      <c r="C52" s="47"/>
+      <c r="A52" s="72"/>
+      <c r="B52" s="73"/>
+      <c r="C52" s="78"/>
       <c r="D52" s="12" t="s">
         <v>7</v>
       </c>
@@ -3463,7 +3781,7 @@
       </c>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="41" t="s">
+      <c r="A53" s="72" t="s">
         <v>8</v>
       </c>
       <c r="B53" s="10" t="s">
@@ -3473,40 +3791,40 @@
         <v>111</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E53" s="10" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="54" spans="1:5" hidden="1">
-      <c r="A54" s="41"/>
+      <c r="A54" s="72"/>
       <c r="B54" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C54" s="43"/>
-      <c r="D54" s="43"/>
+      <c r="C54" s="74"/>
+      <c r="D54" s="74"/>
       <c r="E54" s="10" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:5" hidden="1">
-      <c r="A55" s="41"/>
+      <c r="A55" s="72"/>
       <c r="B55" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="43"/>
-      <c r="D55" s="43"/>
+      <c r="C55" s="74"/>
+      <c r="D55" s="74"/>
       <c r="E55" s="10" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="41"/>
-      <c r="B56" s="42" t="s">
+      <c r="A56" s="72"/>
+      <c r="B56" s="73" t="s">
         <v>61</v>
       </c>
-      <c r="C56" s="42" t="s">
+      <c r="C56" s="73" t="s">
         <v>112</v>
       </c>
       <c r="D56" s="10" t="s">
@@ -3517,9 +3835,9 @@
       </c>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="41"/>
-      <c r="B57" s="42"/>
-      <c r="C57" s="42"/>
+      <c r="A57" s="72"/>
+      <c r="B57" s="73"/>
+      <c r="C57" s="73"/>
       <c r="D57" s="10" t="s">
         <v>7</v>
       </c>
@@ -3528,35 +3846,35 @@
       </c>
     </row>
     <row r="58" spans="1:5" hidden="1">
-      <c r="A58" s="41"/>
+      <c r="A58" s="72"/>
       <c r="B58" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C58" s="43"/>
-      <c r="D58" s="43"/>
+      <c r="C58" s="74"/>
+      <c r="D58" s="74"/>
       <c r="E58" s="10" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="59" spans="1:5" hidden="1">
-      <c r="A59" s="41"/>
+      <c r="A59" s="72"/>
       <c r="B59" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C59" s="43"/>
-      <c r="D59" s="43"/>
+      <c r="C59" s="74"/>
+      <c r="D59" s="74"/>
       <c r="E59" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="44" t="s">
+      <c r="A60" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="B60" s="44" t="s">
+      <c r="B60" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="C60" s="44" t="s">
+      <c r="C60" s="75" t="s">
         <v>113</v>
       </c>
       <c r="D60" s="8" t="s">
@@ -3567,9 +3885,9 @@
       </c>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="44"/>
-      <c r="B61" s="44"/>
-      <c r="C61" s="44"/>
+      <c r="A61" s="75"/>
+      <c r="B61" s="75"/>
+      <c r="C61" s="75"/>
       <c r="D61" s="8" t="s">
         <v>7</v>
       </c>
@@ -3578,72 +3896,72 @@
       </c>
     </row>
     <row r="62" spans="1:5" hidden="1">
-      <c r="A62" s="44"/>
+      <c r="A62" s="75"/>
       <c r="B62" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C62" s="46"/>
-      <c r="D62" s="46"/>
+      <c r="C62" s="77"/>
+      <c r="D62" s="77"/>
       <c r="E62" s="8" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="44" t="s">
+      <c r="A63" s="75" t="s">
         <v>56</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C63" s="46" t="s">
+      <c r="C63" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="D63" s="46"/>
-      <c r="E63" s="46"/>
+      <c r="D63" s="77"/>
+      <c r="E63" s="77"/>
     </row>
     <row r="64" spans="1:5" hidden="1">
-      <c r="A64" s="44"/>
+      <c r="A64" s="75"/>
       <c r="B64" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C64" s="46"/>
-      <c r="D64" s="46"/>
+      <c r="C64" s="77"/>
+      <c r="D64" s="77"/>
       <c r="E64" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="44" t="s">
+      <c r="A65" s="75" t="s">
         <v>65</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C65" s="46" t="s">
+      <c r="C65" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="D65" s="46"/>
-      <c r="E65" s="46"/>
+      <c r="D65" s="77"/>
+      <c r="E65" s="77"/>
     </row>
     <row r="66" spans="1:5" hidden="1">
-      <c r="A66" s="44"/>
+      <c r="A66" s="75"/>
       <c r="B66" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C66" s="46"/>
-      <c r="D66" s="46"/>
+      <c r="C66" s="77"/>
+      <c r="D66" s="77"/>
       <c r="E66" s="8" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="41" t="s">
+      <c r="A67" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="B67" s="42" t="s">
+      <c r="B67" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="C67" s="42" t="s">
+      <c r="C67" s="73" t="s">
         <v>114</v>
       </c>
       <c r="D67" s="10" t="s">
@@ -3654,9 +3972,9 @@
       </c>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="41"/>
-      <c r="B68" s="42"/>
-      <c r="C68" s="42"/>
+      <c r="A68" s="72"/>
+      <c r="B68" s="73"/>
+      <c r="C68" s="73"/>
       <c r="D68" s="10" t="s">
         <v>7</v>
       </c>
@@ -3665,53 +3983,53 @@
       </c>
     </row>
     <row r="69" spans="1:5" hidden="1">
-      <c r="A69" s="41"/>
+      <c r="A69" s="72"/>
       <c r="B69" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C69" s="43"/>
-      <c r="D69" s="43"/>
+      <c r="C69" s="74"/>
+      <c r="D69" s="74"/>
       <c r="E69" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="70" spans="1:5" hidden="1">
-      <c r="A70" s="41"/>
+      <c r="A70" s="72"/>
       <c r="B70" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C70" s="43"/>
-      <c r="D70" s="43"/>
+      <c r="C70" s="74"/>
+      <c r="D70" s="74"/>
       <c r="E70" s="10" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15" customHeight="1">
-      <c r="A71" s="44" t="s">
+      <c r="A71" s="75" t="s">
         <v>45</v>
       </c>
       <c r="B71" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C71" s="45" t="s">
+      <c r="C71" s="76" t="s">
         <v>57</v>
       </c>
-      <c r="D71" s="45"/>
-      <c r="E71" s="45"/>
+      <c r="D71" s="76"/>
+      <c r="E71" s="76"/>
     </row>
     <row r="72" spans="1:5" hidden="1">
-      <c r="A72" s="44"/>
+      <c r="A72" s="75"/>
       <c r="B72" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C72" s="45"/>
-      <c r="D72" s="45"/>
+      <c r="C72" s="76"/>
+      <c r="D72" s="76"/>
       <c r="E72" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="48" t="s">
+      <c r="A73" s="79" t="s">
         <v>71</v>
       </c>
       <c r="B73" s="12" t="s">
@@ -3728,23 +4046,23 @@
       </c>
     </row>
     <row r="74" spans="1:5" hidden="1">
-      <c r="A74" s="48"/>
+      <c r="A74" s="79"/>
       <c r="B74" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C74" s="43"/>
-      <c r="D74" s="43"/>
+      <c r="C74" s="74"/>
+      <c r="D74" s="74"/>
       <c r="E74" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="75" spans="1:5" hidden="1">
-      <c r="A75" s="48"/>
+      <c r="A75" s="79"/>
       <c r="B75" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C75" s="43"/>
-      <c r="D75" s="43"/>
+      <c r="C75" s="74"/>
+      <c r="D75" s="74"/>
       <c r="E75" s="10" t="s">
         <v>74</v>
       </c>
@@ -3856,290 +4174,408 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="55.83203125" customWidth="1"/>
     <col min="2" max="2" width="20.83203125" style="14" customWidth="1"/>
-    <col min="3" max="3" width="55.83203125" style="59" customWidth="1"/>
-    <col min="4" max="4" width="55.83203125" style="60" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="25"/>
+    <col min="3" max="3" width="55.83203125" style="27" customWidth="1"/>
+    <col min="4" max="4" width="55.83203125" style="28" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:4" ht="16" thickBot="1">
+      <c r="A1" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="19" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="30">
+      <c r="A2" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="80" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="81"/>
+      <c r="C3" s="84" t="s">
+        <v>144</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="81"/>
+      <c r="C4" s="84"/>
+      <c r="D4" s="43" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30">
+      <c r="A5" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="81"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="42" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30">
+      <c r="A6" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" s="82" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>148</v>
+      </c>
+      <c r="D6" s="43" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="31" thickBot="1">
+      <c r="A7" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" s="83"/>
+      <c r="C7" s="40" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" s="44" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16" thickBot="1">
+      <c r="A8" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="D1" s="61" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="30">
-      <c r="A2" s="53" t="s">
+      <c r="D8" s="33" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="405" customHeight="1">
+      <c r="A9" s="45" t="s">
+        <v>156</v>
+      </c>
+      <c r="B9" s="85" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="48" t="s">
+        <v>144</v>
+      </c>
+      <c r="D9" s="51" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="36" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10" s="81"/>
+      <c r="C10" s="87" t="s">
+        <v>144</v>
+      </c>
+      <c r="D10" s="87" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="46" t="s">
+        <v>165</v>
+      </c>
+      <c r="B11" s="81"/>
+      <c r="C11" s="87"/>
+      <c r="D11" s="87"/>
+    </row>
+    <row r="12" spans="1:4" ht="240" customHeight="1">
+      <c r="A12" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="B12" s="81" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="49" t="s">
+        <v>162</v>
+      </c>
+      <c r="D12" s="52" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="240" customHeight="1" thickBot="1">
+      <c r="A13" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="B13" s="86"/>
+      <c r="C13" s="50" t="s">
+        <v>159</v>
+      </c>
+      <c r="D13" s="53" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16" thickBot="1">
+      <c r="A14" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="61" t="s">
+        <v>175</v>
+      </c>
+      <c r="B15" s="88" t="s">
+        <v>178</v>
+      </c>
+      <c r="C15" s="91" t="s">
+        <v>139</v>
+      </c>
+      <c r="D15" s="95" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="36" t="s">
+        <v>177</v>
+      </c>
+      <c r="B16" s="89"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="96"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="54" t="s">
+        <v>168</v>
+      </c>
+      <c r="B17" s="89"/>
+      <c r="C17" s="92"/>
+      <c r="D17" s="96"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="36" t="s">
+        <v>174</v>
+      </c>
+      <c r="B18" s="89"/>
+      <c r="C18" s="92"/>
+      <c r="D18" s="96"/>
+    </row>
+    <row r="19" spans="1:4" ht="75">
+      <c r="A19" s="56" t="s">
+        <v>170</v>
+      </c>
+      <c r="B19" s="89"/>
+      <c r="C19" s="92"/>
+      <c r="D19" s="43" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="75" customHeight="1">
+      <c r="A20" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="B20" s="89"/>
+      <c r="C20" s="93" t="s">
+        <v>144</v>
+      </c>
+      <c r="D20" s="57" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16" customHeight="1">
+      <c r="A21" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="B21" s="89"/>
+      <c r="C21" s="93"/>
+      <c r="D21" s="43" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" customHeight="1">
+      <c r="A22" s="36" t="s">
+        <v>166</v>
+      </c>
+      <c r="B22" s="89"/>
+      <c r="C22" s="92" t="s">
+        <v>167</v>
+      </c>
+      <c r="D22" s="57" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" customHeight="1" thickBot="1">
+      <c r="A23" s="62" t="s">
+        <v>169</v>
+      </c>
+      <c r="B23" s="90"/>
+      <c r="C23" s="94"/>
+      <c r="D23" s="43" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" customHeight="1" thickBot="1">
+      <c r="A24" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="B24" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="76" thickBot="1">
+      <c r="A25" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="B25" s="58" t="s">
+        <v>130</v>
+      </c>
+      <c r="C25" s="59" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="D25" s="60"/>
+    </row>
+    <row r="26" spans="1:4" ht="16" thickBot="1">
+      <c r="A26" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="C26" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="D26" s="33" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="58" t="s">
+        <v>133</v>
+      </c>
+      <c r="B27" s="58" t="s">
+        <v>134</v>
+      </c>
+      <c r="C27" s="59"/>
+      <c r="D27" s="60"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="24"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="26"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="24"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="26"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="24"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="26"/>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="C31" s="23"/>
+      <c r="D31" s="26"/>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="B32" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="D2" s="57" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="49" t="s">
-        <v>150</v>
-      </c>
-      <c r="D3" s="56" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="53" t="s">
-        <v>122</v>
-      </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="57" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30">
-      <c r="A5" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="56" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="405" customHeight="1">
-      <c r="A6" s="54" t="s">
-        <v>165</v>
-      </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="58" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="30" t="s">
-        <v>166</v>
-      </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="55" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="54" t="s">
-        <v>174</v>
-      </c>
-      <c r="B8" s="50"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="55"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="24" t="s">
-        <v>162</v>
-      </c>
-      <c r="B9" s="50"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="56"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="B10" s="50"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="56"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="24" t="s">
+      <c r="C32" s="29"/>
+      <c r="D32" s="26"/>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="56" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="24" t="s">
+      <c r="B33" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D33" s="26"/>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="56" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30">
-      <c r="A13" s="53" t="s">
-        <v>153</v>
-      </c>
-      <c r="B13" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>154</v>
-      </c>
-      <c r="D13" s="57" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30">
-      <c r="A14" s="53" t="s">
-        <v>127</v>
-      </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="31" t="s">
-        <v>148</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="24" t="s">
-        <v>129</v>
-      </c>
-      <c r="B15" s="50" t="s">
-        <v>130</v>
-      </c>
-      <c r="C15" s="51" t="s">
-        <v>144</v>
-      </c>
-      <c r="D15" s="56"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="B16" s="50"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="56"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="24" t="s">
-        <v>163</v>
-      </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="56"/>
-    </row>
-    <row r="18" spans="1:4" ht="16" customHeight="1">
-      <c r="A18" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="B18" s="50"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="56"/>
-    </row>
-    <row r="19" spans="1:4" ht="30" customHeight="1">
-      <c r="A19" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="B19" s="50"/>
-      <c r="C19" s="31" t="s">
-        <v>147</v>
-      </c>
-      <c r="D19" s="56"/>
-    </row>
-    <row r="20" spans="1:4" ht="75">
-      <c r="A20" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="C20" s="31" t="s">
-        <v>149</v>
-      </c>
-      <c r="D20" s="56"/>
-    </row>
-    <row r="21" spans="1:4" ht="240" customHeight="1">
-      <c r="A21" s="54" t="s">
-        <v>167</v>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="C21" s="52" t="s">
-        <v>171</v>
-      </c>
-      <c r="D21" s="58" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="240" customHeight="1">
-      <c r="A22" s="54" t="s">
-        <v>164</v>
-      </c>
-      <c r="B22" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="C22" s="52" t="s">
-        <v>168</v>
-      </c>
-      <c r="D22" s="58" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="B23" s="24" t="s">
-        <v>137</v>
-      </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="56"/>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="B24" s="24" t="s">
-        <v>139</v>
-      </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="56"/>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="20"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="62"/>
-    </row>
-    <row r="41" ht="15" customHeight="1"/>
+      <c r="B34" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D34" s="26"/>
+    </row>
+    <row r="48" spans="1:4" ht="15" customHeight="1"/>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="C3:C12"/>
-    <mergeCell ref="B2:B12"/>
-    <mergeCell ref="C15:C18"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="D7:D8"/>
+  <mergeCells count="12">
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="B15:B23"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C10:C11"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
update account service - add cors
</commit_message>
<xml_diff>
--- a/linksPage.xlsx
+++ b/linksPage.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="182">
   <si>
     <t>request</t>
   </si>
@@ -410,9 +410,6 @@
     <t>fullAccountDto</t>
   </si>
   <si>
-    <t>POST /jobSeeker/editVisibility</t>
-  </si>
-  <si>
     <t>fieldsVisibilityDto</t>
   </si>
   <si>
@@ -425,9 +422,6 @@
     <t>POST /company/searchJobSeeker</t>
   </si>
   <si>
-    <t>searchJobSeekerDto</t>
-  </si>
-  <si>
     <t>name request</t>
   </si>
   <si>
@@ -447,12 +441,6 @@
   </si>
   <si>
     <t>structure request</t>
-  </si>
-  <si>
-    <t>{"login":"my@email.com","password":"1234567","typeQuestion":"question1","question":"answerToQuestion","phone":1234567}</t>
-  </si>
-  <si>
-    <t>{"login":"my@email.com","email":true,"firstName":true,"lastName":true,"birthDate":true,"phone":true,"location":true,"photo":true,"aboutMyself":true,"linkedin":true,"educations":true,"languages":true,"coursesAndCertificates":true,"recomendations":true,"experiences":true,"projects":true}</t>
   </si>
   <si>
     <t>{"login":"my@email.com"}</t>
@@ -516,18 +504,9 @@
     <t>"ok" / "wrongRequest" / "exist" / "removed"</t>
   </si>
   <si>
-    <t>"ok" / "noFound" / "removed"</t>
-  </si>
-  <si>
     <t>{"login":"my@Email.com","downloadType":"doc","personData":{"firstName":"name","lastName":"surname","phone":12345671,"location":"rehovot","photoUrl":"http://photoUrl"},"professionalData":{"aboutMySelf":"aboutMySelf","linkedinUrl":"http://linkedinUrl","educations":[{"nameUniversity":"university","nameSpeciality":"speciality","educationDegree":"master","startDate":"2017-12-06","endDate":"2017-12-06"}],"languages":[{"languageName":"english","languageLevel":"basic"}],"coursesAndCertificates":[{"nameOfCourse":"course","endDate":"2017-12-06"}],"recomendations":[{"firstName":"name","lastName":"surname","companyName":"company","position":"position","phone":1234567}],"experiences":[{"companyName":"company1","position":"position1","startDate":"2011-12-06","endDate":"2011-12-06","projects":[{"nameProject":"project1","endDate":"2011-12-06","descriptionProject":"descriptionProject1"}]}]}}</t>
   </si>
   <si>
-    <t>"noFound" / "remove" / "false" {"login":"my@Email.com","downloadType":"doc","curriculumVitae":[{"login":"my@Email.com","yearsInWork":1,"skillsType":["java"],"companyName":["myCompany1"],"verification":{"date":"2017-12-06","verificationStatus":"yes"},"cvType":"backEnd","dateOfEnable":"2017-12-06","enable":true,"minSalary":1}],"personData":{"firstName":"name","lastName":"surname","birthDate":"2017-12-07","phone":1234567,"location":"rehovot","photoUrl":"http://photoUrl"},"professionalData":{"aboutMySelf":"aboutMySelf","linkedinUrl":"http://linkedinUrl","educations":[{"nameUniversity":"university","nameSpeciality":"speciality","educationDegree":"master","startDate":"2017-12-06","endDate":"2017-12-06"}],"languages":[{"languageName":"english","languageLevel":"basic"}],"coursesAndCertificates":[{"nameOfCourse":"course","endDate":"2017-12-06"}],"recomendations":[{"firstName":"name","lastName":"surname","companyName":"company","position":"position","phone":1234567}],"experiences":[{"companyName":"company","position":"position","startDate":"2017-12-06","endDate":"2017-12-06","projects":[{"nameProject":"project","endDate":"2017-12-06","descriptionProject":"descriptionProject"}]}]},"fieldsVisibility":{"login":"my@Email.com","email":true,"firstName":true,"lastName":true,"birthDate":true,"phone":true,"location":true,"photo":true,"aboutMyself":true,"linkedin":true,"educations":true,"languages":true,"coursesAndCertificates":true,"recomendations":true,"experiences":true,"projects":true}}</t>
-  </si>
-  <si>
-    <t>"ok" / "noFound"</t>
-  </si>
-  <si>
     <t>POST /jobSeeker/restoreProfile</t>
   </si>
   <si>
@@ -552,9 +531,6 @@
     <t>"ok" / "wrongRequest" / "noFounf" / "exist"</t>
   </si>
   <si>
-    <t>"noFound" / "ok"</t>
-  </si>
-  <si>
     <t>POST /jobSeeker/deleteCv</t>
   </si>
   <si>
@@ -570,10 +546,37 @@
     <t>jobSeekerCvDto</t>
   </si>
   <si>
-    <t>"noFound" / "false" {"login":"my@Email.com","yearsInWork":1,"skillsType":["java"],"companyName":["myCompany1"],"verification":{"date":"","verificationStatus":"no"},"cvType":"backEnd","dateOfEnable":"2017-12-18","enable":true,"minSalary":1}</t>
-  </si>
-  <si>
-    <t>"noFound" / "false" [{"login":"my@Email.com","yearsInWork":1,"skillsType":["java"],"companyName":["myCompany1"],"verification":{"date":"","verificationStatus":"no"},"cvType":"backEnd","dateOfEnable":"2017-12-18","enable":true,"minSalary":1}]</t>
+    <t>POST /jobSeeker/updateVisibility</t>
+  </si>
+  <si>
+    <t>{"login":"my@Email.com","email":false,"firstName":false,"lastName":false,"birthDate":false,"phone":false,"location":false,"photo":false,"aboutMyself":false,"linkedin":false,"educations":false,"languages":false,"coursesAndCertificates":false,"recomendations":false,"experiences":false,"projects":false}</t>
+  </si>
+  <si>
+    <t>"noFound" / "ok" / "wrongRequest"</t>
+  </si>
+  <si>
+    <t>"noFound" / "false" / "wrongRequest" [{"login":"my@Email.com","yearsInWork":1,"skillsType":["java"],"companyName":["myCompany1"],"verification":{"date":"","verificationStatus":"no"},"cvType":"backEnd","dateOfEnable":"2017-12-18","enable":true,"minSalary":1}]</t>
+  </si>
+  <si>
+    <t>"noFound" / "false" / "wrongRequest" {"login":"my@Email.com","yearsInWork":1,"skillsType":["java"],"companyName":["myCompany1"],"verification":{"date":"","verificationStatus":"no"},"cvType":"backEnd","dateOfEnable":"2017-12-18","enable":true,"minSalary":1}</t>
+  </si>
+  <si>
+    <t>"ok" / "noFound" / "removed" / "wrongRequest"</t>
+  </si>
+  <si>
+    <t>"ok" / "noFound" / "wrongRequest"</t>
+  </si>
+  <si>
+    <t>"noFound" / "remove" / "false" / "wrongRequest" {"login":"my@Email.com","downloadType":"doc","curriculumVitae":[{"login":"my@Email.com","yearsInWork":1,"skillsType":["java"],"companyName":["myCompany1"],"verification":{"date":"2017-12-06","verificationStatus":"yes"},"cvType":"backEnd","dateOfEnable":"2017-12-06","enable":true,"minSalary":1}],"personData":{"firstName":"name","lastName":"surname","birthDate":"2017-12-07","phone":1234567,"location":"rehovot","photoUrl":"http://photoUrl"},"professionalData":{"aboutMySelf":"aboutMySelf","linkedinUrl":"http://linkedinUrl","educations":[{"nameUniversity":"university","nameSpeciality":"speciality","educationDegree":"master","startDate":"2017-12-06","endDate":"2017-12-06"}],"languages":[{"languageName":"english","languageLevel":"basic"}],"coursesAndCertificates":[{"nameOfCourse":"course","endDate":"2017-12-06"}],"recomendations":[{"firstName":"name","lastName":"surname","companyName":"company","position":"position","phone":1234567}],"experiences":[{"companyName":"company","position":"position","startDate":"2017-12-06","endDate":"2017-12-06","projects":[{"nameProject":"project","endDate":"2017-12-06","descriptionProject":"descriptionProject"}]}]},"fieldsVisibility":{"login":"my@Email.com","email":true,"firstName":true,"lastName":true,"birthDate":true,"phone":true,"location":true,"photo":true,"aboutMyself":true,"linkedin":true,"educations":true,"languages":true,"coursesAndCertificates":true,"recomendations":true,"experiences":true,"projects":true}}</t>
+  </si>
+  <si>
+    <t>noFound / "wrongRequest"</t>
+  </si>
+  <si>
+    <t>{"yearsInWork":1,"skillsType":["java"],"verification":{"verificationStatus":"yes"},"cvType":"backEnd","minSalary":1}</t>
+  </si>
+  <si>
+    <t>{"login":"my@email.com","password":"1234567","role":"JOB_SEEKER","typeQuestion":"question1","question":"answerToQuestion","phone":1234567}</t>
   </si>
 </sst>
 </file>
@@ -1278,31 +1281,46 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1311,21 +1329,36 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1348,36 +1381,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="289">
@@ -2052,11 +2055,11 @@
       <c r="A2" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="67" t="s">
-        <v>137</v>
+      <c r="C2" s="64" t="s">
+        <v>135</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>3</v>
@@ -2067,8 +2070,8 @@
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1">
       <c r="A3" s="65"/>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
       <c r="D3" s="15" t="s">
         <v>2</v>
       </c>
@@ -2078,8 +2081,8 @@
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1">
       <c r="A4" s="65"/>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
       <c r="D4" s="15" t="s">
         <v>4</v>
       </c>
@@ -2089,8 +2092,8 @@
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1">
       <c r="A5" s="65"/>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
       <c r="D5" s="15" t="s">
         <v>5</v>
       </c>
@@ -2103,8 +2106,8 @@
       <c r="B6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
       <c r="E6" s="15" t="s">
         <v>18</v>
       </c>
@@ -2139,8 +2142,8 @@
       <c r="B9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
       <c r="E9" s="1" t="s">
         <v>23</v>
       </c>
@@ -2150,8 +2153,8 @@
       <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
       <c r="E10" s="1" t="s">
         <v>28</v>
       </c>
@@ -2175,10 +2178,10 @@
       <c r="A12" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="67" t="s">
+      <c r="B12" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="67" t="s">
+      <c r="C12" s="64" t="s">
         <v>104</v>
       </c>
       <c r="D12" s="15" t="s">
@@ -2190,8 +2193,8 @@
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1">
       <c r="A13" s="65"/>
-      <c r="B13" s="67"/>
-      <c r="C13" s="67"/>
+      <c r="B13" s="64"/>
+      <c r="C13" s="64"/>
       <c r="D13" s="15" t="s">
         <v>5</v>
       </c>
@@ -2201,8 +2204,8 @@
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1">
       <c r="A14" s="65"/>
-      <c r="B14" s="67"/>
-      <c r="C14" s="67"/>
+      <c r="B14" s="64"/>
+      <c r="C14" s="64"/>
       <c r="D14" s="15" t="s">
         <v>7</v>
       </c>
@@ -2217,8 +2220,8 @@
       <c r="B15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
       <c r="E15" s="1" t="s">
         <v>33</v>
       </c>
@@ -2230,8 +2233,8 @@
       <c r="B16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
       <c r="E16" s="1" t="s">
         <v>23</v>
       </c>
@@ -2241,8 +2244,8 @@
       <c r="B17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
       <c r="E17" s="1" t="s">
         <v>33</v>
       </c>
@@ -2265,8 +2268,8 @@
       <c r="B19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="69"/>
-      <c r="D19" s="69"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
       <c r="E19" s="1" t="s">
         <v>33</v>
       </c>
@@ -2293,8 +2296,8 @@
       <c r="B21" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="67"/>
-      <c r="D21" s="67"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="64"/>
       <c r="E21" s="15" t="s">
         <v>77</v>
       </c>
@@ -2304,8 +2307,8 @@
       <c r="B22" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="67"/>
-      <c r="D22" s="67"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="64"/>
       <c r="E22" s="15" t="s">
         <v>50</v>
       </c>
@@ -2315,8 +2318,8 @@
       <c r="B23" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="67"/>
-      <c r="D23" s="67"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="64"/>
       <c r="E23" s="15" t="s">
         <v>84</v>
       </c>
@@ -2326,8 +2329,8 @@
       <c r="B24" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="67"/>
-      <c r="D24" s="67"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="64"/>
       <c r="E24" s="15" t="s">
         <v>33</v>
       </c>
@@ -2337,8 +2340,8 @@
       <c r="B25" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C25" s="63"/>
-      <c r="D25" s="63"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="69"/>
       <c r="E25" s="15" t="s">
         <v>81</v>
       </c>
@@ -2348,8 +2351,8 @@
       <c r="B26" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="63"/>
-      <c r="D26" s="63"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="69"/>
       <c r="E26" s="15" t="s">
         <v>84</v>
       </c>
@@ -2359,18 +2362,18 @@
       <c r="B27" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="63"/>
-      <c r="D27" s="63"/>
+      <c r="C27" s="69"/>
+      <c r="D27" s="69"/>
       <c r="E27" s="15" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" customHeight="1">
       <c r="A28" s="65"/>
-      <c r="B28" s="67" t="s">
+      <c r="B28" s="64" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="67" t="s">
+      <c r="C28" s="64" t="s">
         <v>117</v>
       </c>
       <c r="D28" s="16" t="s">
@@ -2382,8 +2385,8 @@
     </row>
     <row r="29" spans="1:5" ht="15" customHeight="1">
       <c r="A29" s="65"/>
-      <c r="B29" s="67"/>
-      <c r="C29" s="67"/>
+      <c r="B29" s="64"/>
+      <c r="C29" s="64"/>
       <c r="D29" s="15" t="s">
         <v>7</v>
       </c>
@@ -2393,10 +2396,10 @@
     </row>
     <row r="30" spans="1:5" ht="15" customHeight="1">
       <c r="A30" s="65"/>
-      <c r="B30" s="67" t="s">
+      <c r="B30" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="67" t="s">
+      <c r="C30" s="64" t="s">
         <v>118</v>
       </c>
       <c r="D30" s="15" t="s">
@@ -2408,8 +2411,8 @@
     </row>
     <row r="31" spans="1:5" ht="15" customHeight="1">
       <c r="A31" s="65"/>
-      <c r="B31" s="67"/>
-      <c r="C31" s="67"/>
+      <c r="B31" s="64"/>
+      <c r="C31" s="64"/>
       <c r="D31" s="15" t="s">
         <v>7</v>
       </c>
@@ -2419,10 +2422,10 @@
     </row>
     <row r="32" spans="1:5" ht="15" customHeight="1">
       <c r="A32" s="65"/>
-      <c r="B32" s="67" t="s">
+      <c r="B32" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="67" t="s">
+      <c r="C32" s="64" t="s">
         <v>119</v>
       </c>
       <c r="D32" s="15" t="s">
@@ -2434,8 +2437,8 @@
     </row>
     <row r="33" spans="1:5" ht="15" customHeight="1">
       <c r="A33" s="65"/>
-      <c r="B33" s="67"/>
-      <c r="C33" s="67"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="64"/>
       <c r="D33" s="15" t="s">
         <v>7</v>
       </c>
@@ -2476,8 +2479,8 @@
       <c r="B36" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="69"/>
-      <c r="D36" s="69"/>
+      <c r="C36" s="67"/>
+      <c r="D36" s="67"/>
       <c r="E36" s="1" t="s">
         <v>54</v>
       </c>
@@ -2489,19 +2492,19 @@
       <c r="B37" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="69" t="s">
+      <c r="C37" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="69"/>
-      <c r="E37" s="69"/>
+      <c r="D37" s="67"/>
+      <c r="E37" s="67"/>
     </row>
     <row r="38" spans="1:5" ht="15" customHeight="1">
       <c r="A38" s="66"/>
       <c r="B38" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C38" s="69"/>
-      <c r="D38" s="69"/>
+      <c r="C38" s="67"/>
+      <c r="D38" s="67"/>
       <c r="E38" s="1" t="s">
         <v>59</v>
       </c>
@@ -2567,8 +2570,8 @@
       <c r="B43" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C43" s="69"/>
-      <c r="D43" s="69"/>
+      <c r="C43" s="67"/>
+      <c r="D43" s="67"/>
       <c r="E43" s="1" t="s">
         <v>98</v>
       </c>
@@ -2577,10 +2580,10 @@
       <c r="A44" s="65" t="s">
         <v>73</v>
       </c>
-      <c r="B44" s="67" t="s">
+      <c r="B44" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="67" t="s">
+      <c r="C44" s="64" t="s">
         <v>108</v>
       </c>
       <c r="D44" s="15" t="s">
@@ -2592,8 +2595,8 @@
     </row>
     <row r="45" spans="1:5" ht="15" customHeight="1">
       <c r="A45" s="65"/>
-      <c r="B45" s="67"/>
-      <c r="C45" s="67"/>
+      <c r="B45" s="64"/>
+      <c r="C45" s="64"/>
       <c r="D45" s="15" t="s">
         <v>7</v>
       </c>
@@ -2606,8 +2609,8 @@
       <c r="B46" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C46" s="63"/>
-      <c r="D46" s="63"/>
+      <c r="C46" s="69"/>
+      <c r="D46" s="69"/>
       <c r="E46" s="15" t="s">
         <v>33</v>
       </c>
@@ -2617,8 +2620,8 @@
       <c r="B47" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C47" s="63"/>
-      <c r="D47" s="63"/>
+      <c r="C47" s="69"/>
+      <c r="D47" s="69"/>
       <c r="E47" s="15" t="s">
         <v>76</v>
       </c>
@@ -2666,10 +2669,10 @@
     </row>
     <row r="51" spans="1:5" ht="15" customHeight="1">
       <c r="A51" s="65"/>
-      <c r="B51" s="67" t="s">
+      <c r="B51" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="C51" s="71" t="s">
+      <c r="C51" s="63" t="s">
         <v>110</v>
       </c>
       <c r="D51" s="17" t="s">
@@ -2681,8 +2684,8 @@
     </row>
     <row r="52" spans="1:5" ht="15" customHeight="1">
       <c r="A52" s="65"/>
-      <c r="B52" s="67"/>
-      <c r="C52" s="71"/>
+      <c r="B52" s="64"/>
+      <c r="C52" s="63"/>
       <c r="D52" s="17" t="s">
         <v>7</v>
       </c>
@@ -2701,7 +2704,7 @@
         <v>111</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E53" s="15" t="s">
         <v>79</v>
@@ -2712,8 +2715,8 @@
       <c r="B54" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C54" s="63"/>
-      <c r="D54" s="63"/>
+      <c r="C54" s="69"/>
+      <c r="D54" s="69"/>
       <c r="E54" s="15" t="s">
         <v>48</v>
       </c>
@@ -2723,18 +2726,18 @@
       <c r="B55" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="63"/>
-      <c r="D55" s="63"/>
+      <c r="C55" s="69"/>
+      <c r="D55" s="69"/>
       <c r="E55" s="15" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15" customHeight="1">
       <c r="A56" s="65"/>
-      <c r="B56" s="67" t="s">
+      <c r="B56" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="C56" s="67" t="s">
+      <c r="C56" s="64" t="s">
         <v>112</v>
       </c>
       <c r="D56" s="15" t="s">
@@ -2746,8 +2749,8 @@
     </row>
     <row r="57" spans="1:5" ht="15" customHeight="1">
       <c r="A57" s="65"/>
-      <c r="B57" s="67"/>
-      <c r="C57" s="67"/>
+      <c r="B57" s="64"/>
+      <c r="C57" s="64"/>
       <c r="D57" s="15" t="s">
         <v>7</v>
       </c>
@@ -2760,8 +2763,8 @@
       <c r="B58" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C58" s="63"/>
-      <c r="D58" s="63"/>
+      <c r="C58" s="69"/>
+      <c r="D58" s="69"/>
       <c r="E58" s="15" t="s">
         <v>70</v>
       </c>
@@ -2771,8 +2774,8 @@
       <c r="B59" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C59" s="63"/>
-      <c r="D59" s="63"/>
+      <c r="C59" s="69"/>
+      <c r="D59" s="69"/>
       <c r="E59" s="15" t="s">
         <v>33</v>
       </c>
@@ -2810,8 +2813,8 @@
       <c r="B62" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C62" s="69"/>
-      <c r="D62" s="69"/>
+      <c r="C62" s="67"/>
+      <c r="D62" s="67"/>
       <c r="E62" s="1" t="s">
         <v>54</v>
       </c>
@@ -2823,19 +2826,19 @@
       <c r="B63" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C63" s="69" t="s">
+      <c r="C63" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="D63" s="69"/>
-      <c r="E63" s="69"/>
+      <c r="D63" s="67"/>
+      <c r="E63" s="67"/>
     </row>
     <row r="64" spans="1:5" ht="15" customHeight="1">
       <c r="A64" s="66"/>
       <c r="B64" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C64" s="69"/>
-      <c r="D64" s="69"/>
+      <c r="C64" s="67"/>
+      <c r="D64" s="67"/>
       <c r="E64" s="1" t="s">
         <v>59</v>
       </c>
@@ -2847,19 +2850,19 @@
       <c r="B65" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C65" s="69" t="s">
+      <c r="C65" s="67" t="s">
         <v>66</v>
       </c>
-      <c r="D65" s="69"/>
-      <c r="E65" s="69"/>
+      <c r="D65" s="67"/>
+      <c r="E65" s="67"/>
     </row>
     <row r="66" spans="1:5" ht="15" customHeight="1">
       <c r="A66" s="66"/>
       <c r="B66" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C66" s="69"/>
-      <c r="D66" s="69"/>
+      <c r="C66" s="67"/>
+      <c r="D66" s="67"/>
       <c r="E66" s="1" t="s">
         <v>68</v>
       </c>
@@ -2868,10 +2871,10 @@
       <c r="A67" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="B67" s="67" t="s">
+      <c r="B67" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="C67" s="67" t="s">
+      <c r="C67" s="64" t="s">
         <v>114</v>
       </c>
       <c r="D67" s="15" t="s">
@@ -2883,8 +2886,8 @@
     </row>
     <row r="68" spans="1:5" ht="15" customHeight="1">
       <c r="A68" s="65"/>
-      <c r="B68" s="67"/>
-      <c r="C68" s="67"/>
+      <c r="B68" s="64"/>
+      <c r="C68" s="64"/>
       <c r="D68" s="15" t="s">
         <v>7</v>
       </c>
@@ -2897,8 +2900,8 @@
       <c r="B69" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C69" s="63"/>
-      <c r="D69" s="63"/>
+      <c r="C69" s="69"/>
+      <c r="D69" s="69"/>
       <c r="E69" s="15" t="s">
         <v>33</v>
       </c>
@@ -2908,8 +2911,8 @@
       <c r="B70" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C70" s="63"/>
-      <c r="D70" s="63"/>
+      <c r="C70" s="69"/>
+      <c r="D70" s="69"/>
       <c r="E70" s="15" t="s">
         <v>74</v>
       </c>
@@ -2939,7 +2942,7 @@
       </c>
     </row>
     <row r="73" spans="1:5" ht="15" customHeight="1">
-      <c r="A73" s="64" t="s">
+      <c r="A73" s="71" t="s">
         <v>71</v>
       </c>
       <c r="B73" s="17" t="s">
@@ -2956,23 +2959,23 @@
       </c>
     </row>
     <row r="74" spans="1:5" ht="15" customHeight="1">
-      <c r="A74" s="64"/>
+      <c r="A74" s="71"/>
       <c r="B74" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C74" s="63"/>
-      <c r="D74" s="63"/>
+      <c r="C74" s="69"/>
+      <c r="D74" s="69"/>
       <c r="E74" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="15" customHeight="1">
-      <c r="A75" s="64"/>
+      <c r="A75" s="71"/>
       <c r="B75" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C75" s="63"/>
-      <c r="D75" s="63"/>
+      <c r="C75" s="69"/>
+      <c r="D75" s="69"/>
       <c r="E75" s="15" t="s">
         <v>74</v>
       </c>
@@ -3008,27 +3011,56 @@
     <row r="87" spans="3:4" s="2" customFormat="1" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="87">
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="A73:A75"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="A67:A70"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="C44:C45"/>
@@ -3045,56 +3077,27 @@
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="C34:C35"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="A73:A75"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="A67:A70"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:E48"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3138,13 +3141,13 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="78" t="s">
         <v>101</v>
       </c>
       <c r="D2" s="10" t="s">
@@ -3155,9 +3158,9 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="72"/>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
+      <c r="A3" s="77"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="78"/>
       <c r="D3" s="10" t="s">
         <v>2</v>
       </c>
@@ -3166,9 +3169,9 @@
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="72"/>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
+      <c r="A4" s="77"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
       <c r="D4" s="10" t="s">
         <v>4</v>
       </c>
@@ -3177,9 +3180,9 @@
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="72"/>
-      <c r="B5" s="73"/>
-      <c r="C5" s="73"/>
+      <c r="A5" s="77"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
       <c r="D5" s="10" t="s">
         <v>5</v>
       </c>
@@ -3188,31 +3191,31 @@
       </c>
     </row>
     <row r="6" spans="1:5" hidden="1">
-      <c r="A6" s="72"/>
+      <c r="A6" s="77"/>
       <c r="B6" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="74"/>
-      <c r="D6" s="74"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
       <c r="E6" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" hidden="1">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="72" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="76"/>
-      <c r="D7" s="76"/>
-      <c r="E7" s="75" t="s">
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="72" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="75"/>
+      <c r="A8" s="72"/>
       <c r="B8" s="8" t="s">
         <v>24</v>
       </c>
@@ -3220,28 +3223,28 @@
         <v>102</v>
       </c>
       <c r="D8" s="8"/>
-      <c r="E8" s="75"/>
+      <c r="E8" s="72"/>
     </row>
     <row r="9" spans="1:5" hidden="1">
-      <c r="A9" s="75" t="s">
+      <c r="A9" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="77"/>
-      <c r="D9" s="77"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
       <c r="E9" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:5" hidden="1">
-      <c r="A10" s="75"/>
+      <c r="A10" s="72"/>
       <c r="B10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="77"/>
-      <c r="D10" s="77"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
       <c r="E10" s="8" t="s">
         <v>28</v>
       </c>
@@ -3262,13 +3265,13 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="72" t="s">
+      <c r="A12" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="73" t="s">
+      <c r="B12" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="73" t="s">
+      <c r="C12" s="78" t="s">
         <v>104</v>
       </c>
       <c r="D12" s="10" t="s">
@@ -3279,9 +3282,9 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="72"/>
-      <c r="B13" s="73"/>
-      <c r="C13" s="73"/>
+      <c r="A13" s="77"/>
+      <c r="B13" s="78"/>
+      <c r="C13" s="78"/>
       <c r="D13" s="10" t="s">
         <v>5</v>
       </c>
@@ -3290,9 +3293,9 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="72"/>
-      <c r="B14" s="73"/>
-      <c r="C14" s="73"/>
+      <c r="A14" s="77"/>
+      <c r="B14" s="78"/>
+      <c r="C14" s="78"/>
       <c r="D14" s="10" t="s">
         <v>7</v>
       </c>
@@ -3307,62 +3310,62 @@
       <c r="B15" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="77"/>
-      <c r="D15" s="77"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
       <c r="E15" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:5" hidden="1">
-      <c r="A16" s="75" t="s">
+      <c r="A16" s="72" t="s">
         <v>39</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="77"/>
-      <c r="D16" s="77"/>
+      <c r="C16" s="76"/>
+      <c r="D16" s="76"/>
       <c r="E16" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:5" hidden="1">
-      <c r="A17" s="75"/>
+      <c r="A17" s="72"/>
       <c r="B17" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="77"/>
-      <c r="D17" s="77"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="76"/>
       <c r="E17" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1">
-      <c r="A18" s="75" t="s">
+      <c r="A18" s="72" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="76" t="s">
+      <c r="C18" s="73" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="76"/>
-      <c r="E18" s="76"/>
+      <c r="D18" s="73"/>
+      <c r="E18" s="73"/>
     </row>
     <row r="19" spans="1:5" hidden="1">
-      <c r="A19" s="75"/>
+      <c r="A19" s="72"/>
       <c r="B19" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="77"/>
-      <c r="D19" s="77"/>
+      <c r="C19" s="76"/>
+      <c r="D19" s="76"/>
       <c r="E19" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="72" t="s">
+      <c r="A20" s="77" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="10" t="s">
@@ -3379,88 +3382,88 @@
       </c>
     </row>
     <row r="21" spans="1:5" hidden="1">
-      <c r="A21" s="72"/>
+      <c r="A21" s="77"/>
       <c r="B21" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="73"/>
-      <c r="D21" s="73"/>
+      <c r="C21" s="78"/>
+      <c r="D21" s="78"/>
       <c r="E21" s="10" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:5" hidden="1">
-      <c r="A22" s="72"/>
+      <c r="A22" s="77"/>
       <c r="B22" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="73"/>
-      <c r="D22" s="73"/>
+      <c r="C22" s="78"/>
+      <c r="D22" s="78"/>
       <c r="E22" s="10" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:5" hidden="1">
-      <c r="A23" s="72"/>
+      <c r="A23" s="77"/>
       <c r="B23" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="73"/>
-      <c r="D23" s="73"/>
+      <c r="C23" s="78"/>
+      <c r="D23" s="78"/>
       <c r="E23" s="10" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:5" hidden="1">
-      <c r="A24" s="72"/>
+      <c r="A24" s="77"/>
       <c r="B24" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="73"/>
-      <c r="D24" s="73"/>
+      <c r="C24" s="78"/>
+      <c r="D24" s="78"/>
       <c r="E24" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:5" hidden="1">
-      <c r="A25" s="72"/>
+      <c r="A25" s="77"/>
       <c r="B25" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C25" s="74"/>
-      <c r="D25" s="74"/>
+      <c r="C25" s="75"/>
+      <c r="D25" s="75"/>
       <c r="E25" s="10" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:5" hidden="1">
-      <c r="A26" s="72"/>
+      <c r="A26" s="77"/>
       <c r="B26" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="74"/>
-      <c r="D26" s="74"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="75"/>
       <c r="E26" s="10" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:5" hidden="1">
-      <c r="A27" s="72"/>
+      <c r="A27" s="77"/>
       <c r="B27" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="74"/>
-      <c r="D27" s="74"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="75"/>
       <c r="E27" s="10" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="72"/>
-      <c r="B28" s="73" t="s">
+      <c r="A28" s="77"/>
+      <c r="B28" s="78" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="73" t="s">
+      <c r="C28" s="78" t="s">
         <v>117</v>
       </c>
       <c r="D28" s="11" t="s">
@@ -3471,9 +3474,9 @@
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="72"/>
-      <c r="B29" s="73"/>
-      <c r="C29" s="73"/>
+      <c r="A29" s="77"/>
+      <c r="B29" s="78"/>
+      <c r="C29" s="78"/>
       <c r="D29" s="10" t="s">
         <v>7</v>
       </c>
@@ -3482,11 +3485,11 @@
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="72"/>
-      <c r="B30" s="73" t="s">
+      <c r="A30" s="77"/>
+      <c r="B30" s="78" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="73" t="s">
+      <c r="C30" s="78" t="s">
         <v>118</v>
       </c>
       <c r="D30" s="10" t="s">
@@ -3497,9 +3500,9 @@
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="72"/>
-      <c r="B31" s="73"/>
-      <c r="C31" s="73"/>
+      <c r="A31" s="77"/>
+      <c r="B31" s="78"/>
+      <c r="C31" s="78"/>
       <c r="D31" s="10" t="s">
         <v>7</v>
       </c>
@@ -3508,11 +3511,11 @@
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="72"/>
-      <c r="B32" s="73" t="s">
+      <c r="A32" s="77"/>
+      <c r="B32" s="78" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="73" t="s">
+      <c r="C32" s="78" t="s">
         <v>119</v>
       </c>
       <c r="D32" s="10" t="s">
@@ -3523,9 +3526,9 @@
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="72"/>
-      <c r="B33" s="73"/>
-      <c r="C33" s="73"/>
+      <c r="A33" s="77"/>
+      <c r="B33" s="78"/>
+      <c r="C33" s="78"/>
       <c r="D33" s="10" t="s">
         <v>7</v>
       </c>
@@ -3534,13 +3537,13 @@
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="75" t="s">
+      <c r="A34" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="B34" s="75" t="s">
+      <c r="B34" s="72" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="75" t="s">
+      <c r="C34" s="72" t="s">
         <v>106</v>
       </c>
       <c r="D34" s="8" t="s">
@@ -3551,9 +3554,9 @@
       </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="75"/>
-      <c r="B35" s="75"/>
-      <c r="C35" s="75"/>
+      <c r="A35" s="72"/>
+      <c r="B35" s="72"/>
+      <c r="C35" s="72"/>
       <c r="D35" s="8" t="s">
         <v>7</v>
       </c>
@@ -3562,48 +3565,48 @@
       </c>
     </row>
     <row r="36" spans="1:5" hidden="1">
-      <c r="A36" s="75"/>
+      <c r="A36" s="72"/>
       <c r="B36" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="77"/>
-      <c r="D36" s="77"/>
+      <c r="C36" s="76"/>
+      <c r="D36" s="76"/>
       <c r="E36" s="8" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="75" t="s">
+      <c r="A37" s="72" t="s">
         <v>56</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="77" t="s">
+      <c r="C37" s="76" t="s">
         <v>60</v>
       </c>
-      <c r="D37" s="77"/>
-      <c r="E37" s="77"/>
+      <c r="D37" s="76"/>
+      <c r="E37" s="76"/>
     </row>
     <row r="38" spans="1:5" hidden="1">
-      <c r="A38" s="75"/>
+      <c r="A38" s="72"/>
       <c r="B38" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C38" s="77"/>
-      <c r="D38" s="77"/>
+      <c r="C38" s="76"/>
+      <c r="D38" s="76"/>
       <c r="E38" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="75" t="s">
+      <c r="A39" s="72" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="75" t="s">
+      <c r="B39" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="C39" s="75" t="s">
+      <c r="C39" s="72" t="s">
         <v>107</v>
       </c>
       <c r="D39" s="8" t="s">
@@ -3614,9 +3617,9 @@
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="75"/>
-      <c r="B40" s="75"/>
-      <c r="C40" s="75"/>
+      <c r="A40" s="72"/>
+      <c r="B40" s="72"/>
+      <c r="C40" s="72"/>
       <c r="D40" s="8" t="s">
         <v>7</v>
       </c>
@@ -3625,13 +3628,13 @@
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="75" t="s">
+      <c r="A41" s="72" t="s">
         <v>97</v>
       </c>
-      <c r="B41" s="75" t="s">
+      <c r="B41" s="72" t="s">
         <v>52</v>
       </c>
-      <c r="C41" s="75" t="s">
+      <c r="C41" s="72" t="s">
         <v>120</v>
       </c>
       <c r="D41" s="8" t="s">
@@ -3642,9 +3645,9 @@
       </c>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="75"/>
-      <c r="B42" s="75"/>
-      <c r="C42" s="75"/>
+      <c r="A42" s="72"/>
+      <c r="B42" s="72"/>
+      <c r="C42" s="72"/>
       <c r="D42" s="8" t="s">
         <v>7</v>
       </c>
@@ -3653,24 +3656,24 @@
       </c>
     </row>
     <row r="43" spans="1:5" hidden="1">
-      <c r="A43" s="75"/>
+      <c r="A43" s="72"/>
       <c r="B43" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C43" s="77"/>
-      <c r="D43" s="77"/>
+      <c r="C43" s="76"/>
+      <c r="D43" s="76"/>
       <c r="E43" s="8" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="72" t="s">
+      <c r="A44" s="77" t="s">
         <v>73</v>
       </c>
-      <c r="B44" s="73" t="s">
+      <c r="B44" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="C44" s="73" t="s">
+      <c r="C44" s="78" t="s">
         <v>108</v>
       </c>
       <c r="D44" s="10" t="s">
@@ -3681,9 +3684,9 @@
       </c>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="72"/>
-      <c r="B45" s="73"/>
-      <c r="C45" s="73"/>
+      <c r="A45" s="77"/>
+      <c r="B45" s="78"/>
+      <c r="C45" s="78"/>
       <c r="D45" s="10" t="s">
         <v>7</v>
       </c>
@@ -3692,53 +3695,53 @@
       </c>
     </row>
     <row r="46" spans="1:5" hidden="1">
-      <c r="A46" s="72"/>
+      <c r="A46" s="77"/>
       <c r="B46" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C46" s="74"/>
-      <c r="D46" s="74"/>
+      <c r="C46" s="75"/>
+      <c r="D46" s="75"/>
       <c r="E46" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:5" hidden="1">
-      <c r="A47" s="72"/>
+      <c r="A47" s="77"/>
       <c r="B47" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C47" s="74"/>
-      <c r="D47" s="74"/>
+      <c r="C47" s="75"/>
+      <c r="D47" s="75"/>
       <c r="E47" s="10" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15" customHeight="1">
-      <c r="A48" s="75" t="s">
+      <c r="A48" s="72" t="s">
         <v>45</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C48" s="76" t="s">
+      <c r="C48" s="73" t="s">
         <v>57</v>
       </c>
-      <c r="D48" s="76"/>
-      <c r="E48" s="76"/>
+      <c r="D48" s="73"/>
+      <c r="E48" s="73"/>
     </row>
     <row r="49" spans="1:5" hidden="1">
-      <c r="A49" s="75"/>
+      <c r="A49" s="72"/>
       <c r="B49" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="76"/>
-      <c r="D49" s="76"/>
+      <c r="C49" s="73"/>
+      <c r="D49" s="73"/>
       <c r="E49" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="30">
-      <c r="A50" s="72" t="s">
+      <c r="A50" s="77" t="s">
         <v>87</v>
       </c>
       <c r="B50" s="10" t="s">
@@ -3755,11 +3758,11 @@
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="72"/>
-      <c r="B51" s="73" t="s">
+      <c r="A51" s="77"/>
+      <c r="B51" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="C51" s="78" t="s">
+      <c r="C51" s="79" t="s">
         <v>110</v>
       </c>
       <c r="D51" s="12" t="s">
@@ -3770,9 +3773,9 @@
       </c>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="72"/>
-      <c r="B52" s="73"/>
-      <c r="C52" s="78"/>
+      <c r="A52" s="77"/>
+      <c r="B52" s="78"/>
+      <c r="C52" s="79"/>
       <c r="D52" s="12" t="s">
         <v>7</v>
       </c>
@@ -3781,7 +3784,7 @@
       </c>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="72" t="s">
+      <c r="A53" s="77" t="s">
         <v>8</v>
       </c>
       <c r="B53" s="10" t="s">
@@ -3791,40 +3794,40 @@
         <v>111</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E53" s="10" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="54" spans="1:5" hidden="1">
-      <c r="A54" s="72"/>
+      <c r="A54" s="77"/>
       <c r="B54" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C54" s="74"/>
-      <c r="D54" s="74"/>
+      <c r="C54" s="75"/>
+      <c r="D54" s="75"/>
       <c r="E54" s="10" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:5" hidden="1">
-      <c r="A55" s="72"/>
+      <c r="A55" s="77"/>
       <c r="B55" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="74"/>
-      <c r="D55" s="74"/>
+      <c r="C55" s="75"/>
+      <c r="D55" s="75"/>
       <c r="E55" s="10" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="72"/>
-      <c r="B56" s="73" t="s">
+      <c r="A56" s="77"/>
+      <c r="B56" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="C56" s="73" t="s">
+      <c r="C56" s="78" t="s">
         <v>112</v>
       </c>
       <c r="D56" s="10" t="s">
@@ -3835,9 +3838,9 @@
       </c>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="72"/>
-      <c r="B57" s="73"/>
-      <c r="C57" s="73"/>
+      <c r="A57" s="77"/>
+      <c r="B57" s="78"/>
+      <c r="C57" s="78"/>
       <c r="D57" s="10" t="s">
         <v>7</v>
       </c>
@@ -3846,35 +3849,35 @@
       </c>
     </row>
     <row r="58" spans="1:5" hidden="1">
-      <c r="A58" s="72"/>
+      <c r="A58" s="77"/>
       <c r="B58" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C58" s="74"/>
-      <c r="D58" s="74"/>
+      <c r="C58" s="75"/>
+      <c r="D58" s="75"/>
       <c r="E58" s="10" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="59" spans="1:5" hidden="1">
-      <c r="A59" s="72"/>
+      <c r="A59" s="77"/>
       <c r="B59" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C59" s="74"/>
-      <c r="D59" s="74"/>
+      <c r="C59" s="75"/>
+      <c r="D59" s="75"/>
       <c r="E59" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="75" t="s">
+      <c r="A60" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="B60" s="75" t="s">
+      <c r="B60" s="72" t="s">
         <v>52</v>
       </c>
-      <c r="C60" s="75" t="s">
+      <c r="C60" s="72" t="s">
         <v>113</v>
       </c>
       <c r="D60" s="8" t="s">
@@ -3885,9 +3888,9 @@
       </c>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="75"/>
-      <c r="B61" s="75"/>
-      <c r="C61" s="75"/>
+      <c r="A61" s="72"/>
+      <c r="B61" s="72"/>
+      <c r="C61" s="72"/>
       <c r="D61" s="8" t="s">
         <v>7</v>
       </c>
@@ -3896,72 +3899,72 @@
       </c>
     </row>
     <row r="62" spans="1:5" hidden="1">
-      <c r="A62" s="75"/>
+      <c r="A62" s="72"/>
       <c r="B62" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C62" s="77"/>
-      <c r="D62" s="77"/>
+      <c r="C62" s="76"/>
+      <c r="D62" s="76"/>
       <c r="E62" s="8" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="75" t="s">
+      <c r="A63" s="72" t="s">
         <v>56</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C63" s="77" t="s">
+      <c r="C63" s="76" t="s">
         <v>60</v>
       </c>
-      <c r="D63" s="77"/>
-      <c r="E63" s="77"/>
+      <c r="D63" s="76"/>
+      <c r="E63" s="76"/>
     </row>
     <row r="64" spans="1:5" hidden="1">
-      <c r="A64" s="75"/>
+      <c r="A64" s="72"/>
       <c r="B64" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C64" s="77"/>
-      <c r="D64" s="77"/>
+      <c r="C64" s="76"/>
+      <c r="D64" s="76"/>
       <c r="E64" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="75" t="s">
+      <c r="A65" s="72" t="s">
         <v>65</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C65" s="77" t="s">
+      <c r="C65" s="76" t="s">
         <v>66</v>
       </c>
-      <c r="D65" s="77"/>
-      <c r="E65" s="77"/>
+      <c r="D65" s="76"/>
+      <c r="E65" s="76"/>
     </row>
     <row r="66" spans="1:5" hidden="1">
-      <c r="A66" s="75"/>
+      <c r="A66" s="72"/>
       <c r="B66" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C66" s="77"/>
-      <c r="D66" s="77"/>
+      <c r="C66" s="76"/>
+      <c r="D66" s="76"/>
       <c r="E66" s="8" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="72" t="s">
+      <c r="A67" s="77" t="s">
         <v>46</v>
       </c>
-      <c r="B67" s="73" t="s">
+      <c r="B67" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="C67" s="73" t="s">
+      <c r="C67" s="78" t="s">
         <v>114</v>
       </c>
       <c r="D67" s="10" t="s">
@@ -3972,9 +3975,9 @@
       </c>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="72"/>
-      <c r="B68" s="73"/>
-      <c r="C68" s="73"/>
+      <c r="A68" s="77"/>
+      <c r="B68" s="78"/>
+      <c r="C68" s="78"/>
       <c r="D68" s="10" t="s">
         <v>7</v>
       </c>
@@ -3983,53 +3986,53 @@
       </c>
     </row>
     <row r="69" spans="1:5" hidden="1">
-      <c r="A69" s="72"/>
+      <c r="A69" s="77"/>
       <c r="B69" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C69" s="74"/>
-      <c r="D69" s="74"/>
+      <c r="C69" s="75"/>
+      <c r="D69" s="75"/>
       <c r="E69" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="70" spans="1:5" hidden="1">
-      <c r="A70" s="72"/>
+      <c r="A70" s="77"/>
       <c r="B70" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C70" s="74"/>
-      <c r="D70" s="74"/>
+      <c r="C70" s="75"/>
+      <c r="D70" s="75"/>
       <c r="E70" s="10" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15" customHeight="1">
-      <c r="A71" s="75" t="s">
+      <c r="A71" s="72" t="s">
         <v>45</v>
       </c>
       <c r="B71" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C71" s="76" t="s">
+      <c r="C71" s="73" t="s">
         <v>57</v>
       </c>
-      <c r="D71" s="76"/>
-      <c r="E71" s="76"/>
+      <c r="D71" s="73"/>
+      <c r="E71" s="73"/>
     </row>
     <row r="72" spans="1:5" hidden="1">
-      <c r="A72" s="75"/>
+      <c r="A72" s="72"/>
       <c r="B72" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C72" s="76"/>
-      <c r="D72" s="76"/>
+      <c r="C72" s="73"/>
+      <c r="D72" s="73"/>
       <c r="E72" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="79" t="s">
+      <c r="A73" s="74" t="s">
         <v>71</v>
       </c>
       <c r="B73" s="12" t="s">
@@ -4046,78 +4049,51 @@
       </c>
     </row>
     <row r="74" spans="1:5" hidden="1">
-      <c r="A74" s="79"/>
+      <c r="A74" s="74"/>
       <c r="B74" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C74" s="74"/>
-      <c r="D74" s="74"/>
+      <c r="C74" s="75"/>
+      <c r="D74" s="75"/>
       <c r="E74" s="10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="75" spans="1:5" hidden="1">
-      <c r="A75" s="79"/>
+      <c r="A75" s="74"/>
       <c r="B75" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C75" s="74"/>
-      <c r="D75" s="74"/>
+      <c r="C75" s="75"/>
+      <c r="D75" s="75"/>
       <c r="E75" s="10" t="s">
         <v>74</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="87">
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="A73:A75"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="A67:A70"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="A53:A59"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="A41:A43"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:D19"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="C30:C31"/>
     <mergeCell ref="B32:B33"/>
@@ -4134,28 +4110,55 @@
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="C27:D27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A12:A14"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="A53:A59"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="A60:A62"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="A67:A70"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="A73:A75"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
   </mergeCells>
   <conditionalFormatting sqref="A76:E100">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="0">
@@ -4176,8 +4179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4191,319 +4194,325 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16" thickBot="1">
       <c r="A1" s="30" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D1" s="33" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30">
       <c r="A2" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="B2" s="80" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="90" t="s">
         <v>121</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" s="91"/>
+      <c r="C3" s="94" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" s="42" t="s">
         <v>146</v>
-      </c>
-      <c r="B3" s="81"/>
-      <c r="C3" s="84" t="s">
-        <v>144</v>
-      </c>
-      <c r="D3" s="42" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="B4" s="81"/>
-      <c r="C4" s="84"/>
+      <c r="B4" s="91"/>
+      <c r="C4" s="94"/>
       <c r="D4" s="43" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30">
       <c r="A5" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="84"/>
+      <c r="B5" s="91"/>
+      <c r="C5" s="94"/>
       <c r="D5" s="42" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30">
       <c r="A6" s="36" t="s">
-        <v>147</v>
-      </c>
-      <c r="B6" s="82" t="s">
+        <v>143</v>
+      </c>
+      <c r="B6" s="92" t="s">
         <v>128</v>
       </c>
       <c r="C6" s="39" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D6" s="43" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="31" thickBot="1">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="46" thickBot="1">
       <c r="A7" s="37" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="83"/>
+      <c r="B7" s="93"/>
       <c r="C7" s="40" t="s">
-        <v>142</v>
+        <v>181</v>
       </c>
       <c r="D7" s="44" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16" thickBot="1">
       <c r="A8" s="30" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="405" customHeight="1">
       <c r="A9" s="45" t="s">
-        <v>156</v>
-      </c>
-      <c r="B9" s="85" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" s="95" t="s">
         <v>121</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D9" s="51" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="36" t="s">
-        <v>157</v>
-      </c>
-      <c r="B10" s="81"/>
-      <c r="C10" s="87" t="s">
-        <v>144</v>
-      </c>
-      <c r="D10" s="87" t="s">
-        <v>164</v>
+        <v>153</v>
+      </c>
+      <c r="B10" s="91"/>
+      <c r="C10" s="80" t="s">
+        <v>140</v>
+      </c>
+      <c r="D10" s="80" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="46" t="s">
-        <v>165</v>
-      </c>
-      <c r="B11" s="81"/>
-      <c r="C11" s="87"/>
-      <c r="D11" s="87"/>
+        <v>158</v>
+      </c>
+      <c r="B11" s="91"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="80"/>
     </row>
     <row r="12" spans="1:4" ht="240" customHeight="1">
       <c r="A12" s="36" t="s">
-        <v>158</v>
-      </c>
-      <c r="B12" s="81" t="s">
+        <v>154</v>
+      </c>
+      <c r="B12" s="91" t="s">
         <v>100</v>
       </c>
       <c r="C12" s="49" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D12" s="52" t="s">
-        <v>161</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="240" customHeight="1" thickBot="1">
       <c r="A13" s="47" t="s">
+        <v>151</v>
+      </c>
+      <c r="B13" s="96"/>
+      <c r="C13" s="50" t="s">
         <v>155</v>
       </c>
-      <c r="B13" s="86"/>
-      <c r="C13" s="50" t="s">
-        <v>159</v>
-      </c>
       <c r="D13" s="53" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16" thickBot="1">
       <c r="A14" s="30" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D14" s="33" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="61" t="s">
-        <v>175</v>
-      </c>
-      <c r="B15" s="88" t="s">
-        <v>178</v>
-      </c>
-      <c r="C15" s="91" t="s">
-        <v>139</v>
-      </c>
-      <c r="D15" s="95" t="s">
+        <v>167</v>
+      </c>
+      <c r="B15" s="81" t="s">
+        <v>170</v>
+      </c>
+      <c r="C15" s="84" t="s">
+        <v>137</v>
+      </c>
+      <c r="D15" s="88" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="36" t="s">
-        <v>177</v>
-      </c>
-      <c r="B16" s="89"/>
-      <c r="C16" s="92"/>
-      <c r="D16" s="96"/>
+        <v>169</v>
+      </c>
+      <c r="B16" s="82"/>
+      <c r="C16" s="85"/>
+      <c r="D16" s="89"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="54" t="s">
-        <v>168</v>
-      </c>
-      <c r="B17" s="89"/>
-      <c r="C17" s="92"/>
-      <c r="D17" s="96"/>
+        <v>161</v>
+      </c>
+      <c r="B17" s="82"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="89"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="36" t="s">
-        <v>174</v>
-      </c>
-      <c r="B18" s="89"/>
-      <c r="C18" s="92"/>
-      <c r="D18" s="96"/>
+        <v>166</v>
+      </c>
+      <c r="B18" s="82"/>
+      <c r="C18" s="85"/>
+      <c r="D18" s="89"/>
     </row>
     <row r="19" spans="1:4" ht="75">
       <c r="A19" s="56" t="s">
-        <v>170</v>
-      </c>
-      <c r="B19" s="89"/>
-      <c r="C19" s="92"/>
+        <v>163</v>
+      </c>
+      <c r="B19" s="82"/>
+      <c r="C19" s="85"/>
       <c r="D19" s="43" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="75" customHeight="1">
       <c r="A20" s="55" t="s">
-        <v>171</v>
-      </c>
-      <c r="B20" s="89"/>
-      <c r="C20" s="93" t="s">
-        <v>144</v>
+        <v>164</v>
+      </c>
+      <c r="B20" s="82"/>
+      <c r="C20" s="86" t="s">
+        <v>140</v>
       </c>
       <c r="D20" s="57" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16" customHeight="1">
       <c r="A21" s="56" t="s">
-        <v>176</v>
-      </c>
-      <c r="B21" s="89"/>
-      <c r="C21" s="93"/>
+        <v>168</v>
+      </c>
+      <c r="B21" s="82"/>
+      <c r="C21" s="86"/>
       <c r="D21" s="43" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30" customHeight="1">
       <c r="A22" s="36" t="s">
-        <v>166</v>
-      </c>
-      <c r="B22" s="89"/>
-      <c r="C22" s="92" t="s">
-        <v>167</v>
+        <v>159</v>
+      </c>
+      <c r="B22" s="82"/>
+      <c r="C22" s="85" t="s">
+        <v>160</v>
       </c>
       <c r="D22" s="57" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="30" customHeight="1" thickBot="1">
       <c r="A23" s="62" t="s">
-        <v>169</v>
-      </c>
-      <c r="B23" s="90"/>
-      <c r="C23" s="94"/>
+        <v>162</v>
+      </c>
+      <c r="B23" s="83"/>
+      <c r="C23" s="87"/>
       <c r="D23" s="43" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" thickBot="1">
       <c r="A24" s="30" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D24" s="33" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="76" thickBot="1">
       <c r="A25" s="58" t="s">
+        <v>171</v>
+      </c>
+      <c r="B25" s="58" t="s">
         <v>129</v>
       </c>
-      <c r="B25" s="58" t="s">
-        <v>130</v>
-      </c>
       <c r="C25" s="59" t="s">
-        <v>143</v>
-      </c>
-      <c r="D25" s="60"/>
+        <v>172</v>
+      </c>
+      <c r="D25" s="60" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="26" spans="1:4" ht="16" thickBot="1">
       <c r="A26" s="30" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D26" s="33" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="30">
       <c r="A27" s="58" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B27" s="58" t="s">
-        <v>134</v>
-      </c>
-      <c r="C27" s="59"/>
-      <c r="D27" s="60"/>
+        <v>170</v>
+      </c>
+      <c r="C27" s="59" t="s">
+        <v>180</v>
+      </c>
+      <c r="D27" s="60" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="24"/>
@@ -4525,10 +4534,10 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="B31" s="21" t="s">
         <v>131</v>
-      </c>
-      <c r="B31" s="21" t="s">
-        <v>132</v>
       </c>
       <c r="C31" s="23"/>
       <c r="D31" s="26"/>
@@ -4564,18 +4573,18 @@
     <row r="48" spans="1:4" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C10:C11"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="B15:B23"/>
     <mergeCell ref="C15:C19"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="D15:D18"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C10:C11"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>